<commit_message>
tracked len 1 and 3, started 5
</commit_message>
<xml_diff>
--- a/plotting/raw_retake.xlsx
+++ b/plotting/raw_retake.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\GitHub\Togohogo1-Archive\phy180-pendulum-report\plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5942AA00-39B8-4E2B-B068-D6E8998B377D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3774C708-8496-42CE-B777-E4D262315E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="local" sheetId="2" r:id="rId1"/>
+    <sheet name="raw1" sheetId="1" r:id="rId2"/>
+    <sheet name="raw3" sheetId="3" r:id="rId3"/>
+    <sheet name="raw5" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +38,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Kevin Wang</author>
+  </authors>
+  <commentList>
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{C8EE5D0C-85C7-4FA8-947A-09CE8F4B5B33}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kevin Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+if add more decimal places, these values are more precise</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t>t</t>
   </si>
@@ -73,22 +110,77 @@
   <si>
     <t>θf</t>
   </si>
+  <si>
+    <t>h1</t>
+  </si>
+  <si>
+    <t>htop</t>
+  </si>
+  <si>
+    <t>hbot</t>
+  </si>
+  <si>
+    <t>actual len</t>
+  </si>
+  <si>
+    <t>side</t>
+  </si>
+  <si>
+    <t>vid order</t>
+  </si>
+  <si>
+    <t>5  cycles</t>
+  </si>
+  <si>
+    <t>REMEMBER TO DO ANGLE UNCERTAINTY FOR THIS ONE (and maybe others in the future for better best fit lines</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>diff + 1</t>
+  </si>
+  <si>
+    <t>frames</t>
+  </si>
+  <si>
+    <t>sec</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.00000"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,10 +203,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,25 +487,267 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E517E20-6588-4C22-833D-D7D40A2816B4}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4.3</v>
+      </c>
+      <c r="B2">
+        <v>12.4</v>
+      </c>
+      <c r="C2">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D2">
+        <f>(C2+B2)/2-A2</f>
+        <v>10.95</v>
+      </c>
+      <c r="E2">
+        <v>21</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B3">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="C3">
+        <v>23.9</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="0">(C3+B3)/2-A3</f>
+        <v>16.399999999999999</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4.5</v>
+      </c>
+      <c r="B4">
+        <v>22.4</v>
+      </c>
+      <c r="C4">
+        <v>28.1</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>20.75</v>
+      </c>
+      <c r="E4">
+        <f>21*2</f>
+        <v>42</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.5</v>
+      </c>
+      <c r="B5">
+        <v>25.9</v>
+      </c>
+      <c r="C5">
+        <v>31.7</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>24.299999999999997</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4.5</v>
+      </c>
+      <c r="B6">
+        <v>31.8</v>
+      </c>
+      <c r="C6">
+        <v>37.4</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>30.1</v>
+      </c>
+      <c r="E6">
+        <f>21*3</f>
+        <v>63</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4.5</v>
+      </c>
+      <c r="B7">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="C7">
+        <v>41.9</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>34.599999999999994</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4.5</v>
+      </c>
+      <c r="B8">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="C8">
+        <v>46.6</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>39.200000000000003</v>
+      </c>
+      <c r="E8">
+        <v>48</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4.5</v>
+      </c>
+      <c r="B9">
+        <v>44.5</v>
+      </c>
+      <c r="C9">
+        <v>50.1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>42.8</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4.5</v>
+      </c>
+      <c r="B10">
+        <v>50.4</v>
+      </c>
+      <c r="C10">
+        <v>56.2</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>48.8</v>
+      </c>
+      <c r="E10">
+        <f>21*5</f>
+        <v>105</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:P22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -423,7 +758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -467,7 +802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>218</v>
       </c>
@@ -512,12 +847,12 @@
         <f>1/30</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P3" s="2">
-        <f>0.01</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P3" s="3">
+        <f>RADIANS((D3-H3)/2)</f>
+        <v>1.4351842439149345E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>668</v>
       </c>
@@ -562,12 +897,12 @@
         <f t="shared" ref="O4:O22" si="4">1/30</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P4" s="2">
-        <f t="shared" ref="P4:P22" si="5">0.01</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P4" s="3">
+        <f t="shared" ref="P4:P22" si="5">RADIANS((D4-H4)/2)</f>
+        <v>1.1623020153656276E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1116</v>
       </c>
@@ -612,12 +947,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.2941616403537989E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1564</v>
       </c>
@@ -659,12 +994,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.4474015486788911E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2011</v>
       </c>
@@ -710,12 +1045,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.210734902108466E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2458</v>
       </c>
@@ -761,12 +1096,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+        <v>8.4583018874775408E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2924</v>
       </c>
@@ -812,12 +1147,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.0399020749232673E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3370</v>
       </c>
@@ -859,12 +1194,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.0561510902593208E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3815</v>
       </c>
@@ -906,12 +1241,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.202793654011901E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4260</v>
       </c>
@@ -953,12 +1288,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.0931957036329024E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4725</v>
       </c>
@@ -1000,12 +1335,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.0450595228629105E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>5169</v>
       </c>
@@ -1047,12 +1382,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.0450071629853465E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>5612</v>
       </c>
@@ -1094,12 +1429,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+        <v>9.5215564677925378E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>6076</v>
       </c>
@@ -1141,12 +1476,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+        <v>8.0088796050889633E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>6518</v>
       </c>
@@ -1188,12 +1523,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+        <v>9.6359628002607445E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>6961</v>
       </c>
@@ -1235,12 +1570,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P18" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+        <v>9.5386606944620547E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>7422</v>
       </c>
@@ -1282,12 +1617,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P19" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.0139490289461083E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>7863</v>
       </c>
@@ -1329,12 +1664,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P20" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+        <v>9.2080953341343186E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>8325</v>
       </c>
@@ -1376,12 +1711,12 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P21" s="2">
+      <c r="P21" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+        <v>8.8325877455676001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>8765</v>
       </c>
@@ -1423,13 +1758,900 @@
         <f t="shared" si="4"/>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P22" s="2">
+      <c r="P22" s="3">
         <f t="shared" si="5"/>
-        <v>0.01</v>
+        <v>9.4666658628172543E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>239</v>
+      </c>
+      <c r="C27">
+        <v>341</v>
+      </c>
+      <c r="D27">
+        <f>C27-B27+1</f>
+        <v>103</v>
+      </c>
+      <c r="E27">
+        <f>D27/5</f>
+        <v>20.6</v>
+      </c>
+      <c r="F27">
+        <f>E27*(1/30)</f>
+        <v>0.68666666666666676</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D974DD-495F-47A9-A253-4B7C907EF0C3}">
+  <dimension ref="A1:O26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="1"/>
+    <col min="13" max="13" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>209</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-116.94450000000001</v>
+      </c>
+      <c r="D3" s="1">
+        <f>-90-C3</f>
+        <v>26.944500000000005</v>
+      </c>
+      <c r="E3" s="1">
+        <v>209</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-114.502</v>
+      </c>
+      <c r="H3" s="1">
+        <f>-90-G3</f>
+        <v>24.501999999999995</v>
+      </c>
+      <c r="I3" s="1">
+        <v>349.63409999999999</v>
+      </c>
+      <c r="J3" s="1">
+        <v>-92.580399999999997</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <f>RADIANS((H3+D3)/2)</f>
+        <v>0.44895540681363139</v>
+      </c>
+      <c r="N3" s="2">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O3" s="2">
+        <f>RADIANS((D3-H3)/2)</f>
+        <v>2.1314833489980835E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1152</v>
+      </c>
+      <c r="B4" s="1">
+        <v>31.436409999999999</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-112.212</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D17" si="0">-90-C4</f>
+        <v>22.212000000000003</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1152</v>
+      </c>
+      <c r="F4" s="1">
+        <v>31.436409999999999</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-110.3867</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H17" si="1">-90-G4</f>
+        <v>20.386700000000005</v>
+      </c>
+      <c r="I4" s="1">
+        <v>350.0675</v>
+      </c>
+      <c r="J4" s="1">
+        <v>-86.599530000000001</v>
+      </c>
+      <c r="L4" s="2">
+        <v>31.436409999999999</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" ref="M4:M17" si="2">RADIANS((H4+D4)/2)</f>
+        <v>0.3717437860346543</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N17" si="3">1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" ref="O4:O17" si="4">RADIANS((D4-H4)/2)</f>
+        <v>1.5928747418326235E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2065</v>
+      </c>
+      <c r="B5" s="1">
+        <v>61.872709999999998</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-108.11499999999999</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>18.114999999999995</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2065</v>
+      </c>
+      <c r="F5" s="1">
+        <v>61.872709999999998</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-106.654</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>16.653999999999996</v>
+      </c>
+      <c r="L5" s="2">
+        <v>61.872709999999998</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="2"/>
+        <v>0.30341676381295413</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="4"/>
+        <v>1.2749630185818565E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3003</v>
+      </c>
+      <c r="B6" s="1">
+        <v>93.142430000000004</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-104.999</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>14.998999999999995</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3003</v>
+      </c>
+      <c r="F6" s="1">
+        <v>93.142430000000004</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-103.7617</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>13.761700000000005</v>
+      </c>
+      <c r="I6" s="1">
+        <f>-90-J3</f>
+        <v>2.5803999999999974</v>
+      </c>
+      <c r="L6" s="2">
+        <v>93.142430000000004</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="2"/>
+        <v>0.25098445508916656</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0797479417462837E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3940</v>
+      </c>
+      <c r="B7" s="1">
+        <v>124.3788</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-102.3805</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>12.380499999999998</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3940</v>
+      </c>
+      <c r="F7" s="1">
+        <v>124.3788</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-101.1401</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>11.140100000000004</v>
+      </c>
+      <c r="I7" s="1">
+        <f>-90-J4</f>
+        <v>-3.4004699999999985</v>
+      </c>
+      <c r="L7" s="2">
+        <v>124.3788</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="2"/>
+        <v>0.20525595602228916</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="4"/>
+        <v>1.0824532020868778E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>4848</v>
+      </c>
+      <c r="B8" s="1">
+        <v>154.64840000000001</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-100.6737</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>10.673699999999997</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4848</v>
+      </c>
+      <c r="F8" s="1">
+        <v>154.64840000000001</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-98.820239999999998</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>8.8202399999999983</v>
+      </c>
+      <c r="I8" s="1">
+        <f>AVERAGE(I6:I7)</f>
+        <v>-0.41003500000000059</v>
+      </c>
+      <c r="L8" s="2">
+        <v>154.64840000000001</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="2"/>
+        <v>0.17011671859311167</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="4"/>
+        <v>1.6174489777007035E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>5783</v>
+      </c>
+      <c r="B9" s="1">
+        <v>185.81809999999999</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-98.71754</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>8.7175399999999996</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5783</v>
+      </c>
+      <c r="F9" s="1">
+        <v>185.81809999999999</v>
+      </c>
+      <c r="G9" s="1">
+        <v>-96.968429999999998</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>6.9684299999999979</v>
+      </c>
+      <c r="L9" s="2">
+        <v>185.81809999999999</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.13688591143452744</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="4"/>
+        <v>1.5263864239779023E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>6718</v>
+      </c>
+      <c r="B10" s="1">
+        <v>216.9879</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-96.862099999999998</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>6.8620999999999981</v>
+      </c>
+      <c r="E10" s="1">
+        <v>6718</v>
+      </c>
+      <c r="F10" s="1">
+        <v>216.9879</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-95.231269999999995</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>5.231269999999995</v>
+      </c>
+      <c r="L10" s="2">
+        <v>216.9879</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="2"/>
+        <v>0.10553456208095327</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="4"/>
+        <v>1.4231676520149589E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>7651</v>
+      </c>
+      <c r="B11" s="1">
+        <v>248.0909</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-95.655289999999994</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>5.6552899999999937</v>
+      </c>
+      <c r="E11" s="1">
+        <v>7651</v>
+      </c>
+      <c r="F11" s="1">
+        <v>248.0909</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-94.067139999999995</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>4.0671399999999949</v>
+      </c>
+      <c r="L11" s="2">
+        <v>248.0909</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="2"/>
+        <v>8.4844207397336044E-2</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="4"/>
+        <v>1.3859223257773962E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>8585</v>
+      </c>
+      <c r="B12" s="1">
+        <v>279.22730000000001</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-94.553129999999996</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>4.5531299999999959</v>
+      </c>
+      <c r="E12" s="1">
+        <v>8585</v>
+      </c>
+      <c r="F12" s="1">
+        <v>279.22730000000001</v>
+      </c>
+      <c r="G12" s="1">
+        <v>-92.842119999999994</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8421199999999942</v>
+      </c>
+      <c r="L12" s="2">
+        <v>279.22730000000001</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="2"/>
+        <v>6.4535730754055248E-2</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="4"/>
+        <v>1.4931379017274104E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>9517</v>
+      </c>
+      <c r="B13" s="1">
+        <v>310.29700000000003</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-93.678049999999999</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6780499999999989</v>
+      </c>
+      <c r="E13" s="1">
+        <v>9517</v>
+      </c>
+      <c r="F13" s="1">
+        <v>310.29700000000003</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-91.807839999999999</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8078399999999988</v>
+      </c>
+      <c r="L13" s="2">
+        <v>310.29700000000003</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="2"/>
+        <v>4.7873421451115845E-2</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="4"/>
+        <v>1.6320661101861575E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>10450</v>
+      </c>
+      <c r="B14" s="1">
+        <v>341.4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-92.732560000000007</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7325600000000065</v>
+      </c>
+      <c r="E14" s="1">
+        <v>10450</v>
+      </c>
+      <c r="F14" s="1">
+        <v>341.4</v>
+      </c>
+      <c r="G14" s="1">
+        <v>-91.158690000000007</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1586900000000071</v>
+      </c>
+      <c r="L14" s="2">
+        <v>341.4</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="2"/>
+        <v>3.3957562259114796E-2</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="4"/>
+        <v>1.3734606749181573E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>11382</v>
+      </c>
+      <c r="B15" s="1">
+        <v>372.46969999999999</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-92.219840000000005</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2198400000000049</v>
+      </c>
+      <c r="E15" s="1">
+        <v>11382</v>
+      </c>
+      <c r="F15" s="1">
+        <v>372.46969999999999</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-90.313109999999995</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.31310999999999467</v>
+      </c>
+      <c r="L15" s="2">
+        <v>372.46969999999999</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="2"/>
+        <v>2.2104158644195182E-2</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="4"/>
+        <v>1.6639358223275828E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>12313</v>
+      </c>
+      <c r="B16" s="1">
+        <v>403.5061</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-91.532889999999995</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5328899999999948</v>
+      </c>
+      <c r="E16" s="1">
+        <v>12313</v>
+      </c>
+      <c r="F16" s="1">
+        <v>403.5061</v>
+      </c>
+      <c r="G16" s="1">
+        <v>-90.181560000000005</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.18156000000000461</v>
+      </c>
+      <c r="L16" s="2">
+        <v>403.5061</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="2"/>
+        <v>1.4961398680408387E-2</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="4"/>
+        <v>1.1792578890487401E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>13244</v>
+      </c>
+      <c r="B17" s="1">
+        <v>434.54239999999999</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-91.433279999999996</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4332799999999963</v>
+      </c>
+      <c r="E17" s="1">
+        <v>13244</v>
+      </c>
+      <c r="F17" s="1">
+        <v>434.54239999999999</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-90.126490000000004</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.12649000000000399</v>
+      </c>
+      <c r="L17" s="2">
+        <v>434.54239999999999</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="2"/>
+        <v>1.361156103691598E-2</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="4"/>
+        <v>1.1403894066068282E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>1057</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1612</v>
+      </c>
+      <c r="D26" s="1">
+        <f>(C26-B26)+1</f>
+        <v>556</v>
+      </c>
+      <c r="E26" s="1">
+        <f>D26/5</f>
+        <v>111.2</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*(1/120)</f>
+        <v>0.92666666666666664</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C06E64-4DD0-4156-BBC7-DA1C59AF4F60}">
+  <dimension ref="B24:F26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>420</v>
+      </c>
+      <c r="C26" s="1">
+        <v>586</v>
+      </c>
+      <c r="D26" s="1">
+        <f>(C26-B26)+1</f>
+        <v>167</v>
+      </c>
+      <c r="E26" s="1">
+        <f>D26/5</f>
+        <v>33.4</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*(1/30)</f>
+        <v>1.1133333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
done len 5 7 8 (q factor graph starting to look legit)
</commit_message>
<xml_diff>
--- a/plotting/raw_retake.xlsx
+++ b/plotting/raw_retake.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\GitHub\Togohogo1-Archive\phy180-pendulum-report\plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3774C708-8496-42CE-B777-E4D262315E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390BBB18-60E5-4185-B876-B26A2088B80D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="local" sheetId="2" r:id="rId1"/>
-    <sheet name="raw1" sheetId="1" r:id="rId2"/>
-    <sheet name="raw3" sheetId="3" r:id="rId3"/>
-    <sheet name="raw5" sheetId="4" r:id="rId4"/>
+    <sheet name="len1" sheetId="1" r:id="rId2"/>
+    <sheet name="len3" sheetId="3" r:id="rId3"/>
+    <sheet name="len5" sheetId="4" r:id="rId4"/>
+    <sheet name="len7" sheetId="5" r:id="rId5"/>
+    <sheet name="len8" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="33">
   <si>
     <t>t</t>
   </si>
@@ -152,16 +154,38 @@
   <si>
     <t>sec</t>
   </si>
+  <si>
+    <t>per</t>
+  </si>
+  <si>
+    <t>len</t>
+  </si>
+  <si>
+    <t>interm</t>
+  </si>
+  <si>
+    <t>right offset</t>
+  </si>
+  <si>
+    <t>left offset</t>
+  </si>
+  <si>
+    <t>offset left</t>
+  </si>
+  <si>
+    <t>thetaf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +205,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,11 +234,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,13 +523,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E517E20-6588-4C22-833D-D7D40A2816B4}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -516,7 +549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4.3</v>
       </c>
@@ -540,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4.5999999999999996</v>
       </c>
@@ -561,7 +594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4.5</v>
       </c>
@@ -586,7 +619,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4.5</v>
       </c>
@@ -607,7 +640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4.5</v>
       </c>
@@ -632,7 +665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4.5</v>
       </c>
@@ -653,7 +686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4.5</v>
       </c>
@@ -677,7 +710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4.5</v>
       </c>
@@ -698,7 +731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>4.5</v>
       </c>
@@ -732,22 +765,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="M2" sqref="M2:P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -758,7 +791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -802,7 +835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>218</v>
       </c>
@@ -833,15 +866,15 @@
         <v>9</v>
       </c>
       <c r="K3">
-        <f>(H3+D3)/2+I9</f>
-        <v>20.551984999999995</v>
+        <f>(H3+D3)/2-$I$9</f>
+        <v>20.947814999999999</v>
       </c>
       <c r="M3" s="2">
         <v>0</v>
       </c>
       <c r="N3" s="2">
         <f>RADIANS(K3)</f>
-        <v>0.35869980607048674</v>
+        <v>0.36560834284865595</v>
       </c>
       <c r="O3" s="2">
         <f>1/30</f>
@@ -852,7 +885,7 @@
         <v>1.4351842439149345E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>668</v>
       </c>
@@ -883,15 +916,15 @@
         <v>-90.562989999999999</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K22" si="2">(H4+D4)/2+I10</f>
-        <v>18.476350000000004</v>
+        <f t="shared" ref="K4:K22" si="2">(H4+D4)/2-$I$9</f>
+        <v>18.674265000000005</v>
       </c>
       <c r="M4" s="2">
         <v>15.001469999999999</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" ref="N4:N22" si="3">RADIANS(K4)</f>
-        <v>0.32247314125085436</v>
+        <v>0.32592740963993899</v>
       </c>
       <c r="O4" s="2">
         <f t="shared" ref="O4:O22" si="4">1/30</f>
@@ -902,7 +935,7 @@
         <v>1.1623020153656276E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1116</v>
       </c>
@@ -934,14 +967,14 @@
       </c>
       <c r="K5">
         <f t="shared" si="2"/>
-        <v>15.655299999999997</v>
+        <v>15.853214999999999</v>
       </c>
       <c r="M5" s="2">
         <v>29.936260000000001</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" si="3"/>
-        <v>0.2732365303874682</v>
+        <v>0.27669079877655284</v>
       </c>
       <c r="O5" s="2">
         <f t="shared" si="4"/>
@@ -952,7 +985,7 @@
         <v>1.2941616403537989E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1564</v>
       </c>
@@ -979,16 +1012,19 @@
         <f t="shared" si="1"/>
         <v>12.455200000000005</v>
       </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
       <c r="K6">
         <f t="shared" si="2"/>
-        <v>13.284500000000001</v>
+        <v>13.482415000000003</v>
       </c>
       <c r="M6" s="2">
         <v>44.871040000000001</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" si="3"/>
-        <v>0.23185826448118674</v>
+        <v>0.23531253287027135</v>
       </c>
       <c r="O6" s="2">
         <f t="shared" si="4"/>
@@ -999,7 +1035,7 @@
         <v>1.4474015486788911E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2011</v>
       </c>
@@ -1032,14 +1068,14 @@
       </c>
       <c r="K7">
         <f t="shared" si="2"/>
-        <v>11.182499999999997</v>
+        <v>11.380414999999999</v>
       </c>
       <c r="M7" s="2">
         <v>59.772500000000001</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" si="3"/>
-        <v>0.19517144360426586</v>
+        <v>0.19862571199335047</v>
       </c>
       <c r="O7" s="2">
         <f t="shared" si="4"/>
@@ -1050,7 +1086,7 @@
         <v>1.210734902108466E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2458</v>
       </c>
@@ -1083,14 +1119,14 @@
       </c>
       <c r="K8">
         <f t="shared" si="2"/>
-        <v>9.2879050000000021</v>
+        <v>9.4858200000000039</v>
       </c>
       <c r="M8" s="2">
         <v>74.673959999999994</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="3"/>
-        <v>0.16210452286244398</v>
+        <v>0.16555879125152859</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="4"/>
@@ -1101,7 +1137,7 @@
         <v>8.4583018874775408E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2924</v>
       </c>
@@ -1134,14 +1170,14 @@
       </c>
       <c r="K9">
         <f t="shared" si="2"/>
-        <v>7.559820000000002</v>
+        <v>7.7577350000000038</v>
       </c>
       <c r="M9" s="2">
         <v>90.20881</v>
       </c>
       <c r="N9" s="2">
         <f t="shared" si="3"/>
-        <v>0.13194374985811777</v>
+        <v>0.13539801824720238</v>
       </c>
       <c r="O9" s="2">
         <f t="shared" si="4"/>
@@ -1152,7 +1188,7 @@
         <v>1.0399020749232673E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>3370</v>
       </c>
@@ -1181,14 +1217,14 @@
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>5.8234899999999996</v>
+        <v>6.0214050000000015</v>
       </c>
       <c r="M10" s="2">
         <v>105.07689999999999</v>
       </c>
       <c r="N10" s="2">
         <f t="shared" si="3"/>
-        <v>0.10163907445696457</v>
+        <v>0.10509334284604918</v>
       </c>
       <c r="O10" s="2">
         <f t="shared" si="4"/>
@@ -1199,7 +1235,7 @@
         <v>1.0561510902593208E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>3815</v>
       </c>
@@ -1228,14 +1264,14 @@
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>4.8060699999999983</v>
+        <v>5.0039850000000001</v>
       </c>
       <c r="M11" s="2">
         <v>119.9117</v>
       </c>
       <c r="N11" s="2">
         <f t="shared" si="3"/>
-        <v>8.3881745581323844E-2</v>
+        <v>8.7336013970408452E-2</v>
       </c>
       <c r="O11" s="2">
         <f t="shared" si="4"/>
@@ -1246,7 +1282,7 @@
         <v>1.202793654011901E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>4260</v>
       </c>
@@ -1275,14 +1311,14 @@
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
-        <v>3.6099850000000018</v>
+        <v>3.8079000000000036</v>
       </c>
       <c r="M12" s="2">
         <v>134.7465</v>
       </c>
       <c r="N12" s="2">
         <f t="shared" si="3"/>
-        <v>6.3006124197607524E-2</v>
+        <v>6.6460392586692132E-2</v>
       </c>
       <c r="O12" s="2">
         <f t="shared" si="4"/>
@@ -1293,7 +1329,7 @@
         <v>1.0931957036329024E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>4725</v>
       </c>
@@ -1322,14 +1358,14 @@
       </c>
       <c r="K13">
         <f t="shared" si="2"/>
-        <v>2.9625350000000026</v>
+        <v>3.1604500000000044</v>
       </c>
       <c r="M13" s="2">
         <v>150.24799999999999</v>
       </c>
       <c r="N13" s="2">
         <f t="shared" si="3"/>
-        <v>5.1705989955570256E-2</v>
+        <v>5.5160258344654864E-2</v>
       </c>
       <c r="O13" s="2">
         <f t="shared" si="4"/>
@@ -1340,7 +1376,7 @@
         <v>1.0450595228629105E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>5169</v>
       </c>
@@ -1369,14 +1405,14 @@
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>1.998624999999997</v>
+        <v>2.1965399999999988</v>
       </c>
       <c r="M14" s="2">
         <v>165.04949999999999</v>
       </c>
       <c r="N14" s="2">
         <f t="shared" si="3"/>
-        <v>3.4882586762671614E-2</v>
+        <v>3.8336855151756229E-2</v>
       </c>
       <c r="O14" s="2">
         <f t="shared" si="4"/>
@@ -1387,7 +1423,7 @@
         <v>1.0450071629853465E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>5612</v>
       </c>
@@ -1416,14 +1452,14 @@
       </c>
       <c r="K15">
         <f t="shared" si="2"/>
-        <v>1.5063049999999976</v>
+        <v>1.7042199999999994</v>
       </c>
       <c r="M15" s="2">
         <v>179.8176</v>
       </c>
       <c r="N15" s="2">
         <f t="shared" si="3"/>
-        <v>2.6289981789253142E-2</v>
+        <v>2.9744250178337754E-2</v>
       </c>
       <c r="O15" s="2">
         <f t="shared" si="4"/>
@@ -1434,7 +1470,7 @@
         <v>9.5215564677925378E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>6076</v>
       </c>
@@ -1463,14 +1499,14 @@
       </c>
       <c r="K16">
         <f t="shared" si="2"/>
-        <v>1.1698850000000007</v>
+        <v>1.3678000000000026</v>
       </c>
       <c r="M16" s="2">
         <v>195.28569999999999</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" si="3"/>
-        <v>2.0418345119693874E-2</v>
+        <v>2.3872613508778485E-2</v>
       </c>
       <c r="O16" s="2">
         <f t="shared" si="4"/>
@@ -1481,7 +1517,7 @@
         <v>8.0088796050889633E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>6518</v>
       </c>
@@ -1510,14 +1546,14 @@
       </c>
       <c r="K17">
         <f t="shared" si="2"/>
-        <v>0.84763000000000233</v>
+        <v>1.0455450000000042</v>
       </c>
       <c r="M17" s="2">
         <v>210.0205</v>
       </c>
       <c r="N17" s="2">
         <f t="shared" si="3"/>
-        <v>1.4793934338679576E-2</v>
+        <v>1.8248202727764187E-2</v>
       </c>
       <c r="O17" s="2">
         <f t="shared" si="4"/>
@@ -1528,7 +1564,7 @@
         <v>9.6359628002607445E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>6961</v>
       </c>
@@ -1557,14 +1593,14 @@
       </c>
       <c r="K18">
         <f t="shared" si="2"/>
-        <v>0.74537499999999568</v>
+        <v>0.94328999999999752</v>
       </c>
       <c r="M18" s="2">
         <v>224.7886</v>
       </c>
       <c r="N18" s="2">
         <f t="shared" si="3"/>
-        <v>1.3009247912052659E-2</v>
+        <v>1.6463516301137269E-2</v>
       </c>
       <c r="O18" s="2">
         <f t="shared" si="4"/>
@@ -1575,7 +1611,7 @@
         <v>9.5386606944620547E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>7422</v>
       </c>
@@ -1604,14 +1640,14 @@
       </c>
       <c r="K19">
         <f t="shared" si="2"/>
-        <v>0.5184899999999999</v>
+        <v>0.71640500000000173</v>
       </c>
       <c r="M19" s="2">
         <v>240.1568</v>
       </c>
       <c r="N19" s="2">
         <f t="shared" si="3"/>
-        <v>9.0493576386653975E-3</v>
+        <v>1.2503626027750007E-2</v>
       </c>
       <c r="O19" s="2">
         <f t="shared" si="4"/>
@@ -1622,7 +1658,7 @@
         <v>1.0139490289461083E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>7863</v>
       </c>
@@ -1651,14 +1687,14 @@
       </c>
       <c r="K20">
         <f t="shared" si="2"/>
-        <v>0.47120499999999765</v>
+        <v>0.66911999999999949</v>
       </c>
       <c r="M20" s="2">
         <v>254.85820000000001</v>
       </c>
       <c r="N20" s="2">
         <f t="shared" si="3"/>
-        <v>8.2240787018598403E-3</v>
+        <v>1.1678347090944449E-2</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" si="4"/>
@@ -1669,7 +1705,7 @@
         <v>9.2080953341343186E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>8325</v>
       </c>
@@ -1698,14 +1734,14 @@
       </c>
       <c r="K21">
         <f t="shared" si="2"/>
-        <v>0.37075000000000102</v>
+        <v>0.56866500000000286</v>
       </c>
       <c r="M21" s="2">
         <v>270.25970000000001</v>
       </c>
       <c r="N21" s="2">
         <f t="shared" si="3"/>
-        <v>6.4708082017689945E-3</v>
+        <v>9.9250765908536036E-3</v>
       </c>
       <c r="O21" s="2">
         <f t="shared" si="4"/>
@@ -1716,7 +1752,7 @@
         <v>8.8325877455676001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>8765</v>
       </c>
@@ -1745,14 +1781,14 @@
       </c>
       <c r="K22">
         <f t="shared" si="2"/>
-        <v>0.30420999999999765</v>
+        <v>0.50212499999999949</v>
       </c>
       <c r="M22" s="2">
         <v>284.92779999999999</v>
       </c>
       <c r="N22" s="2">
         <f t="shared" si="3"/>
-        <v>5.3094661174919091E-3</v>
+        <v>8.763734506576519E-3</v>
       </c>
       <c r="O22" s="2">
         <f t="shared" si="4"/>
@@ -1763,12 +1799,12 @@
         <v>9.4666658628172543E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>239</v>
       </c>
@@ -1788,7 +1824,7 @@
         <v>0.68666666666666676</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>19</v>
       </c>
@@ -1802,29 +1838,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D974DD-495F-47A9-A253-4B7C907EF0C3}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:F26"/>
+      <selection activeCell="M2" sqref="M2:P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="1"/>
-    <col min="13" max="13" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="1"/>
+    <col min="9" max="9" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.26953125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="9.1796875" style="1"/>
+    <col min="14" max="14" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1838,7 +1875,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1863,20 +1900,23 @@
       <c r="J2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>209</v>
       </c>
@@ -1909,23 +1949,27 @@
       <c r="J3" s="1">
         <v>-92.580399999999997</v>
       </c>
-      <c r="L3" s="2">
+      <c r="K3" s="1">
+        <f>(D3+H3)/2-$I$8</f>
+        <v>26.133285000000001</v>
+      </c>
+      <c r="M3" s="2">
         <v>0</v>
       </c>
-      <c r="M3" s="2">
-        <f>RADIANS((H3+D3)/2)</f>
-        <v>0.44895540681363139</v>
-      </c>
       <c r="N3" s="2">
+        <f>RADIANS(K3)</f>
+        <v>0.45611186761204636</v>
+      </c>
+      <c r="O3" s="2">
         <f>1/30</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <f>RADIANS((D3-H3)/2)</f>
         <v>2.1314833489980835E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1152</v>
       </c>
@@ -1958,23 +2002,27 @@
       <c r="J4" s="1">
         <v>-86.599530000000001</v>
       </c>
-      <c r="L4" s="2">
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:K17" si="2">(D4+H4)/2-$I$8</f>
+        <v>21.709385000000005</v>
+      </c>
+      <c r="M4" s="2">
         <v>31.436409999999999</v>
       </c>
-      <c r="M4" s="2">
-        <f t="shared" ref="M4:M17" si="2">RADIANS((H4+D4)/2)</f>
-        <v>0.3717437860346543</v>
-      </c>
       <c r="N4" s="2">
-        <f t="shared" ref="N4:N17" si="3">1/30</f>
-        <v>3.3333333333333333E-2</v>
+        <f t="shared" ref="N4:N17" si="3">RADIANS(K4)</f>
+        <v>0.37890024683306928</v>
       </c>
       <c r="O4" s="2">
-        <f t="shared" ref="O4:O17" si="4">RADIANS((D4-H4)/2)</f>
+        <f t="shared" ref="O4:O17" si="4">1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" ref="P4:P17" si="5">RADIANS((D4-H4)/2)</f>
         <v>1.5928747418326235E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2065</v>
       </c>
@@ -2001,23 +2049,30 @@
         <f t="shared" si="1"/>
         <v>16.653999999999996</v>
       </c>
-      <c r="L5" s="2">
+      <c r="J5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="2"/>
+        <v>17.794534999999996</v>
+      </c>
+      <c r="M5" s="2">
         <v>61.872709999999998</v>
       </c>
-      <c r="M5" s="2">
-        <f t="shared" si="2"/>
-        <v>0.30341676381295413</v>
-      </c>
       <c r="N5" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>0.3105732246113691</v>
       </c>
       <c r="O5" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="5"/>
         <v>1.2749630185818565E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>3003</v>
       </c>
@@ -2048,23 +2103,27 @@
         <f>-90-J3</f>
         <v>2.5803999999999974</v>
       </c>
-      <c r="L6" s="2">
+      <c r="K6" s="1">
+        <f t="shared" si="2"/>
+        <v>14.790385000000001</v>
+      </c>
+      <c r="M6" s="2">
         <v>93.142430000000004</v>
       </c>
-      <c r="M6" s="2">
-        <f t="shared" si="2"/>
-        <v>0.25098445508916656</v>
-      </c>
       <c r="N6" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>0.25814091588758153</v>
       </c>
       <c r="O6" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="5"/>
         <v>1.0797479417462837E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3940</v>
       </c>
@@ -2095,23 +2154,27 @@
         <f>-90-J4</f>
         <v>-3.4004699999999985</v>
       </c>
-      <c r="L7" s="2">
+      <c r="K7" s="1">
+        <f t="shared" si="2"/>
+        <v>12.170335000000001</v>
+      </c>
+      <c r="M7" s="2">
         <v>124.3788</v>
       </c>
-      <c r="M7" s="2">
-        <f t="shared" si="2"/>
-        <v>0.20525595602228916</v>
-      </c>
       <c r="N7" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>0.21241241682070411</v>
       </c>
       <c r="O7" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="5"/>
         <v>1.0824532020868778E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>4848</v>
       </c>
@@ -2142,23 +2205,27 @@
         <f>AVERAGE(I6:I7)</f>
         <v>-0.41003500000000059</v>
       </c>
-      <c r="L8" s="2">
+      <c r="K8" s="1">
+        <f t="shared" si="2"/>
+        <v>10.157004999999998</v>
+      </c>
+      <c r="M8" s="2">
         <v>154.64840000000001</v>
       </c>
-      <c r="M8" s="2">
-        <f t="shared" si="2"/>
-        <v>0.17011671859311167</v>
-      </c>
       <c r="N8" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>0.17727317939152662</v>
       </c>
       <c r="O8" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="5"/>
         <v>1.6174489777007035E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>5783</v>
       </c>
@@ -2185,23 +2252,27 @@
         <f t="shared" si="1"/>
         <v>6.9684299999999979</v>
       </c>
-      <c r="L9" s="2">
+      <c r="K9" s="1">
+        <f t="shared" si="2"/>
+        <v>8.2530199999999994</v>
+      </c>
+      <c r="M9" s="2">
         <v>185.81809999999999</v>
       </c>
-      <c r="M9" s="2">
-        <f t="shared" si="2"/>
-        <v>0.13688591143452744</v>
-      </c>
       <c r="N9" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>0.14404237223294242</v>
       </c>
       <c r="O9" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="5"/>
         <v>1.5263864239779023E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>6718</v>
       </c>
@@ -2228,23 +2299,27 @@
         <f t="shared" si="1"/>
         <v>5.231269999999995</v>
       </c>
-      <c r="L10" s="2">
+      <c r="K10" s="1">
+        <f t="shared" si="2"/>
+        <v>6.4567199999999971</v>
+      </c>
+      <c r="M10" s="2">
         <v>216.9879</v>
       </c>
-      <c r="M10" s="2">
-        <f t="shared" si="2"/>
-        <v>0.10553456208095327</v>
-      </c>
       <c r="N10" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>0.11269102287936822</v>
       </c>
       <c r="O10" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="5"/>
         <v>1.4231676520149589E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>7651</v>
       </c>
@@ -2271,23 +2346,27 @@
         <f t="shared" si="1"/>
         <v>4.0671399999999949</v>
       </c>
-      <c r="L11" s="2">
+      <c r="K11" s="1">
+        <f t="shared" si="2"/>
+        <v>5.2712499999999949</v>
+      </c>
+      <c r="M11" s="2">
         <v>248.0909</v>
       </c>
-      <c r="M11" s="2">
-        <f t="shared" si="2"/>
-        <v>8.4844207397336044E-2</v>
-      </c>
       <c r="N11" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>9.2000668195751006E-2</v>
       </c>
       <c r="O11" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="5"/>
         <v>1.3859223257773962E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>8585</v>
       </c>
@@ -2314,23 +2393,27 @@
         <f t="shared" si="1"/>
         <v>2.8421199999999942</v>
       </c>
-      <c r="L12" s="2">
+      <c r="K12" s="1">
+        <f t="shared" si="2"/>
+        <v>4.1076599999999956</v>
+      </c>
+      <c r="M12" s="2">
         <v>279.22730000000001</v>
       </c>
-      <c r="M12" s="2">
-        <f t="shared" si="2"/>
-        <v>6.4535730754055248E-2</v>
-      </c>
       <c r="N12" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>7.1692191552470197E-2</v>
       </c>
       <c r="O12" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="5"/>
         <v>1.4931379017274104E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>9517</v>
       </c>
@@ -2357,23 +2440,27 @@
         <f t="shared" si="1"/>
         <v>1.8078399999999988</v>
       </c>
-      <c r="L13" s="2">
+      <c r="K13" s="1">
+        <f t="shared" si="2"/>
+        <v>3.1529799999999994</v>
+      </c>
+      <c r="M13" s="2">
         <v>310.29700000000003</v>
       </c>
-      <c r="M13" s="2">
-        <f t="shared" si="2"/>
-        <v>4.7873421451115845E-2</v>
-      </c>
       <c r="N13" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>5.5029882249530801E-2</v>
       </c>
       <c r="O13" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="5"/>
         <v>1.6320661101861575E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>10450</v>
       </c>
@@ -2400,23 +2487,27 @@
         <f t="shared" si="1"/>
         <v>1.1586900000000071</v>
       </c>
-      <c r="L14" s="2">
+      <c r="K14" s="1">
+        <f t="shared" si="2"/>
+        <v>2.3556600000000074</v>
+      </c>
+      <c r="M14" s="2">
         <v>341.4</v>
       </c>
-      <c r="M14" s="2">
-        <f t="shared" si="2"/>
-        <v>3.3957562259114796E-2</v>
-      </c>
       <c r="N14" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>4.1114023057529751E-2</v>
       </c>
       <c r="O14" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="5"/>
         <v>1.3734606749181573E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>11382</v>
       </c>
@@ -2443,23 +2534,27 @@
         <f t="shared" si="1"/>
         <v>0.31310999999999467</v>
       </c>
-      <c r="L15" s="2">
+      <c r="K15" s="1">
+        <f t="shared" si="2"/>
+        <v>1.6765100000000004</v>
+      </c>
+      <c r="M15" s="2">
         <v>372.46969999999999</v>
       </c>
-      <c r="M15" s="2">
-        <f t="shared" si="2"/>
-        <v>2.2104158644195182E-2</v>
-      </c>
       <c r="N15" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>2.9260619442610141E-2</v>
       </c>
       <c r="O15" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="5"/>
         <v>1.6639358223275828E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>12313</v>
       </c>
@@ -2486,23 +2581,27 @@
         <f t="shared" si="1"/>
         <v>0.18156000000000461</v>
       </c>
-      <c r="L16" s="2">
+      <c r="K16" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2672600000000003</v>
+      </c>
+      <c r="M16" s="2">
         <v>403.5061</v>
       </c>
-      <c r="M16" s="2">
-        <f t="shared" si="2"/>
-        <v>1.4961398680408387E-2</v>
-      </c>
       <c r="N16" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>2.2117859478823346E-2</v>
       </c>
       <c r="O16" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="5"/>
         <v>1.1792578890487401E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>13244</v>
       </c>
@@ -2529,28 +2628,32 @@
         <f t="shared" si="1"/>
         <v>0.12649000000000399</v>
       </c>
-      <c r="L17" s="2">
+      <c r="K17" s="1">
+        <f t="shared" si="2"/>
+        <v>1.1899200000000008</v>
+      </c>
+      <c r="M17" s="2">
         <v>434.54239999999999</v>
       </c>
-      <c r="M17" s="2">
-        <f t="shared" si="2"/>
-        <v>1.361156103691598E-2</v>
-      </c>
       <c r="N17" s="2">
         <f t="shared" si="3"/>
-        <v>3.3333333333333333E-2</v>
+        <v>2.0768021835330941E-2</v>
       </c>
       <c r="O17" s="2">
         <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="5"/>
         <v>1.1403894066068282E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
@@ -2567,7 +2670,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B26" s="1">
         <v>1057</v>
       </c>
@@ -2594,18 +2697,1748 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C06E64-4DD0-4156-BBC7-DA1C59AF4F60}">
-  <dimension ref="B24:F26"/>
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="1"/>
+    <col min="9" max="10" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.08984375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>387</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-116.1</v>
+      </c>
+      <c r="D3" s="1">
+        <f>-90-C3</f>
+        <v>26.099999999999994</v>
+      </c>
+      <c r="E3" s="1">
+        <v>387</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-111.2265</v>
+      </c>
+      <c r="H3" s="1">
+        <f>-90-G3</f>
+        <v>21.226500000000001</v>
+      </c>
+      <c r="I3" s="1">
+        <v>389.10469999999998</v>
+      </c>
+      <c r="J3" s="1">
+        <v>389.10469999999998</v>
+      </c>
+      <c r="K3" s="1">
+        <v>-92.870909999999995</v>
+      </c>
+      <c r="L3" s="1">
+        <f>(D3+H3)/2+$J$8</f>
+        <v>23.811115000000001</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <f>RADIANS((D3+H3)/2+M8)</f>
+        <v>0.41300162422254816</v>
+      </c>
+      <c r="P3" s="2">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>RADIANS(-(H3-D3)/2)</f>
+        <v>4.2529310547971766E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>1482</v>
+      </c>
+      <c r="B4" s="1">
+        <v>36.50356</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-110.4461</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D18" si="0">-90-C4</f>
+        <v>20.446100000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1482</v>
+      </c>
+      <c r="F4" s="1">
+        <v>36.50356</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-106.2457</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H18" si="1">-90-G4</f>
+        <v>16.245699999999999</v>
+      </c>
+      <c r="I4" s="1">
+        <v>389.63799999999998</v>
+      </c>
+      <c r="J4" s="1">
+        <v>389.63799999999998</v>
+      </c>
+      <c r="K4" s="1">
+        <v>-86.833359999999999</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" ref="L4:L18" si="2">(D4+H4)/2+$J$8</f>
+        <v>18.493765000000003</v>
+      </c>
+      <c r="N4" s="2">
+        <v>36.50356</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" ref="O4:O18" si="3">RADIANS((D4+H4)/2+M9)</f>
+        <v>0.3201963592416277</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" ref="P4:P18" si="4">1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q4" s="2">
+        <f t="shared" ref="Q4:Q18" si="5">RADIANS(-(H4-D4)/2)</f>
+        <v>3.6655404950384926E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>2540</v>
+      </c>
+      <c r="B5" s="1">
+        <v>71.773669999999996</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-106.4515</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>16.451499999999996</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2540</v>
+      </c>
+      <c r="F5" s="1">
+        <v>71.773669999999996</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-102.92919999999999</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>12.929199999999994</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="2"/>
+        <v>14.838214999999998</v>
+      </c>
+      <c r="N5" s="2">
+        <v>71.773669999999996</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="3"/>
+        <v>0.25639497577034892</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q5" s="2">
+        <f t="shared" si="5"/>
+        <v>3.0737866121498147E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>3630</v>
+      </c>
+      <c r="B6" s="1">
+        <v>108.11060000000001</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-103.2831</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>13.283100000000005</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3631</v>
+      </c>
+      <c r="F6" s="1">
+        <v>108.1439</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-100.3259</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>10.325900000000004</v>
+      </c>
+      <c r="J6" s="1">
+        <f>90+K4</f>
+        <v>3.166640000000001</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="2"/>
+        <v>11.952365000000007</v>
+      </c>
+      <c r="N6" s="2">
+        <v>108.11060000000001</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="3"/>
+        <v>0.20602739155167071</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" si="5"/>
+        <v>2.5806438319988158E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>4719</v>
+      </c>
+      <c r="B7" s="1">
+        <v>144.41409999999999</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-101.0262</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>11.026200000000003</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4719</v>
+      </c>
+      <c r="F7" s="1">
+        <v>144.41409999999999</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-98.633210000000005</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>8.6332100000000054</v>
+      </c>
+      <c r="J7" s="1">
+        <f>90+K3</f>
+        <v>-2.870909999999995</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="2"/>
+        <v>9.9775700000000072</v>
+      </c>
+      <c r="N7" s="2">
+        <v>144.41409999999999</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="3"/>
+        <v>0.17156071674974929</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="5"/>
+        <v>2.0882777233649532E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>5807</v>
+      </c>
+      <c r="B8" s="1">
+        <v>180.68430000000001</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-99.089079999999996</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>9.0890799999999956</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5807</v>
+      </c>
+      <c r="F8" s="1">
+        <v>180.68430000000001</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-96.799490000000006</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>6.7994900000000058</v>
+      </c>
+      <c r="J8" s="1">
+        <f>AVERAGE(J6:J7)</f>
+        <v>0.14786500000000302</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="2"/>
+        <v>8.0921500000000037</v>
+      </c>
+      <c r="N8" s="2">
+        <v>180.68430000000001</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="3"/>
+        <v>0.13865392996679773</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="5"/>
+        <v>1.9980442010368395E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>6860</v>
+      </c>
+      <c r="B9" s="1">
+        <v>215.7877</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-97.491219999999998</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>7.4912199999999984</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6860</v>
+      </c>
+      <c r="F9" s="1">
+        <v>215.7877</v>
+      </c>
+      <c r="G9" s="1">
+        <v>-95.656170000000003</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>5.656170000000003</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="2"/>
+        <v>6.7215600000000038</v>
+      </c>
+      <c r="N9" s="2">
+        <v>215.7877</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="3"/>
+        <v>0.11473262177188866</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="5"/>
+        <v>1.6013832219360931E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>7947</v>
+      </c>
+      <c r="B10" s="1">
+        <v>252.02459999999999</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-96.186719999999994</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>6.186719999999994</v>
+      </c>
+      <c r="E10" s="1">
+        <v>7947</v>
+      </c>
+      <c r="F10" s="1">
+        <v>252.02459999999999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-94.428610000000006</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>4.4286100000000062</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="2"/>
+        <v>5.4555300000000031</v>
+      </c>
+      <c r="N10" s="2">
+        <v>252.02459999999999</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="3"/>
+        <v>9.2636229842864834E-2</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5342404056118648E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>9033</v>
+      </c>
+      <c r="B11" s="1">
+        <v>288.22809999999998</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-94.867170000000002</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8671700000000016</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9033</v>
+      </c>
+      <c r="F11" s="1">
+        <v>288.22809999999998</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-93.551810000000003</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5518100000000032</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="2"/>
+        <v>4.3573550000000054</v>
+      </c>
+      <c r="N11" s="2">
+        <v>288.22809999999998</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="3"/>
+        <v>7.3469460329776151E-2</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="5"/>
+        <v>1.1478681424516291E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>10120</v>
+      </c>
+      <c r="B12" s="1">
+        <v>324.46499999999997</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-93.991240000000005</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>3.9912400000000048</v>
+      </c>
+      <c r="E12" s="1">
+        <v>10121</v>
+      </c>
+      <c r="F12" s="1">
+        <v>324.49829999999997</v>
+      </c>
+      <c r="G12" s="1">
+        <v>-92.217950000000002</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>2.2179500000000019</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="2"/>
+        <v>3.2524600000000063</v>
+      </c>
+      <c r="N12" s="2">
+        <v>324.46499999999997</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="3"/>
+        <v>5.4185404690953412E-2</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5474874546345149E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>11204</v>
+      </c>
+      <c r="B13" s="1">
+        <v>360.6019</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-93.417119999999997</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>3.417119999999997</v>
+      </c>
+      <c r="E13" s="1">
+        <v>11204</v>
+      </c>
+      <c r="F13" s="1">
+        <v>360.6019</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-91.690259999999995</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.690259999999995</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="2"/>
+        <v>2.701554999999999</v>
+      </c>
+      <c r="N13" s="2">
+        <v>360.6019</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="3"/>
+        <v>4.4570298575253922E-2</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="5"/>
+        <v>1.5069696360494657E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>12290</v>
+      </c>
+      <c r="B14" s="1">
+        <v>396.80540000000002</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-92.886269999999996</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8862699999999961</v>
+      </c>
+      <c r="E14" s="1">
+        <v>12290</v>
+      </c>
+      <c r="F14" s="1">
+        <v>396.80540000000002</v>
+      </c>
+      <c r="G14" s="1">
+        <v>-91.313270000000003</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.3132700000000028</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="2"/>
+        <v>2.2476350000000025</v>
+      </c>
+      <c r="N14" s="2">
+        <v>396.80540000000002</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="3"/>
+        <v>3.6647900034601326E-2</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="5"/>
+        <v>1.3727014566935343E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>13375</v>
+      </c>
+      <c r="B15" s="1">
+        <v>432.97559999999999</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-92.288820000000001</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2888200000000012</v>
+      </c>
+      <c r="E15" s="1">
+        <v>13376</v>
+      </c>
+      <c r="F15" s="1">
+        <v>433.00889999999998</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-91.077650000000006</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.0776500000000055</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="2"/>
+        <v>1.8311000000000064</v>
+      </c>
+      <c r="N15" s="2">
+        <v>432.97559999999999</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="3"/>
+        <v>2.9377992834806813E-2</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q15" s="2">
+        <f t="shared" si="5"/>
+        <v>1.0569452150689822E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>14425</v>
+      </c>
+      <c r="B16" s="1">
+        <v>467.97899999999998</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-91.873390000000001</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8733900000000006</v>
+      </c>
+      <c r="E16" s="1">
+        <v>14425</v>
+      </c>
+      <c r="F16" s="1">
+        <v>467.97899999999998</v>
+      </c>
+      <c r="G16" s="1">
+        <v>-90.442390000000003</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.44239000000000317</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="2"/>
+        <v>1.3057550000000049</v>
+      </c>
+      <c r="N16" s="2">
+        <v>467.97899999999998</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="3"/>
+        <v>2.0208992875917174E-2</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="5"/>
+        <v>1.2487830798019406E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>15511</v>
+      </c>
+      <c r="B17" s="1">
+        <v>504.18259999999998</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-91.682829999999996</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6828299999999956</v>
+      </c>
+      <c r="E17" s="1">
+        <v>15510</v>
+      </c>
+      <c r="F17" s="1">
+        <v>504.14920000000001</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-90.376379999999997</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.37637999999999749</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="2"/>
+        <v>1.1774699999999996</v>
+      </c>
+      <c r="N17" s="2">
+        <v>504.18259999999998</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="3"/>
+        <v>1.7969997244996157E-2</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q17" s="2">
+        <f t="shared" si="5"/>
+        <v>1.1400927006339942E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>16199</v>
+      </c>
+      <c r="B18" s="1">
+        <v>527.11810000000003</v>
+      </c>
+      <c r="C18" s="1">
+        <v>-91.639949999999999</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6399499999999989</v>
+      </c>
+      <c r="E18" s="1">
+        <v>16200</v>
+      </c>
+      <c r="F18" s="1">
+        <v>527.15150000000006</v>
+      </c>
+      <c r="G18" s="1">
+        <v>-90.179739999999995</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.17973999999999535</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0577100000000002</v>
+      </c>
+      <c r="N18" s="2">
+        <v>527.11810000000003</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="3"/>
+        <v>1.5879790932807756E-2</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" si="5"/>
+        <v>1.2742736135273231E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B26" s="1">
+        <v>420</v>
+      </c>
+      <c r="C26" s="1">
+        <v>586</v>
+      </c>
+      <c r="D26" s="1">
+        <f>(C26-B26)+1</f>
+        <v>167</v>
+      </c>
+      <c r="E26" s="1">
+        <f>D26/5</f>
+        <v>33.4</v>
+      </c>
+      <c r="F26" s="1">
+        <f>E26*(1/30)</f>
+        <v>1.1133333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00982F54-7457-4B6E-ABC3-446903AE64B5}">
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>96</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-114.44750000000001</v>
+      </c>
+      <c r="D3" s="1">
+        <f>-90-C3</f>
+        <v>24.447500000000005</v>
+      </c>
+      <c r="E3" s="1">
+        <v>96</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-107.2881</v>
+      </c>
+      <c r="H3" s="1">
+        <f>-G3-90</f>
+        <v>17.2881</v>
+      </c>
+      <c r="I3" s="1">
+        <v>428.29180000000002</v>
+      </c>
+      <c r="J3" s="1">
+        <v>-86.859290000000001</v>
+      </c>
+      <c r="K3">
+        <f>(D3+H3)/2+$I$8</f>
+        <v>21.582149999999999</v>
+      </c>
+      <c r="M3" s="2">
+        <f>F3</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <f>RADIANS(K3)</f>
+        <v>0.37667957715929418</v>
+      </c>
+      <c r="O3" s="2">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P3" s="2">
+        <f>RADIANS((D3-H3)/2)</f>
+        <v>6.2477551233641057E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>1344</v>
+      </c>
+      <c r="B4" s="1">
+        <v>41.587389999999999</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-108.1712</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D16" si="0">-90-C4</f>
+        <v>18.171199999999999</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1344</v>
+      </c>
+      <c r="F4" s="1">
+        <v>41.587389999999999</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-102.3082</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H17" si="1">-G4-90</f>
+        <v>12.308199999999999</v>
+      </c>
+      <c r="I4" s="1">
+        <v>428.89190000000002</v>
+      </c>
+      <c r="J4" s="1">
+        <v>-91.712010000000006</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K17" si="2">(D4+H4)/2+$I$8</f>
+        <v>15.954049999999995</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" ref="M4:M17" si="3">F4</f>
+        <v>41.587389999999999</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N17" si="4">RADIANS(K4)</f>
+        <v>0.27845070152780127</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" ref="O4:O17" si="5">1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" ref="P4:P17" si="6">RADIANS((D4-H4)/2)</f>
+        <v>5.1164327022213768E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>2627</v>
+      </c>
+      <c r="B5" s="1">
+        <v>84.358230000000006</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-103.9875</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>13.987499999999997</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2627</v>
+      </c>
+      <c r="F5" s="1">
+        <v>84.358230000000006</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-99.090209999999999</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>9.090209999999999</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>12.253204999999994</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="3"/>
+        <v>84.358230000000006</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="4"/>
+        <v>0.21385877117183169</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" si="6"/>
+        <v>4.2736917462496533E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>3869</v>
+      </c>
+      <c r="B6" s="1">
+        <v>125.7623</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-100.9876</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>10.9876</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3869</v>
+      </c>
+      <c r="F6" s="1">
+        <v>125.7623</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-96.949269999999999</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>6.9492699999999985</v>
+      </c>
+      <c r="I6" s="1">
+        <f>180+J3-90</f>
+        <v>3.1407099999999986</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>9.6827849999999955</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="3"/>
+        <v>125.7623</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="4"/>
+        <v>0.16899647901271905</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="6"/>
+        <v>3.5241077391031321E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>5149</v>
+      </c>
+      <c r="B7" s="1">
+        <v>168.4331</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-98.548720000000003</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>8.548720000000003</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5149</v>
+      </c>
+      <c r="F7" s="1">
+        <v>168.4331</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-95.157640000000001</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>5.1576400000000007</v>
+      </c>
+      <c r="I7" s="1">
+        <f>180+J4-90</f>
+        <v>-1.7120100000000065</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>7.5675299999999979</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="3"/>
+        <v>168.4331</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="4"/>
+        <v>0.13207831474344645</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="6"/>
+        <v>2.9592755599264674E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>6390</v>
+      </c>
+      <c r="B8" s="1">
+        <v>209.8038</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-96.711619999999996</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>6.7116199999999964</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6390</v>
+      </c>
+      <c r="F8" s="1">
+        <v>209.8038</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-93.899339999999995</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>3.8993399999999951</v>
+      </c>
+      <c r="I8" s="1">
+        <f>(I7+I6)/2</f>
+        <v>0.71434999999999604</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>6.0198299999999918</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="3"/>
+        <v>209.8038</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="4"/>
+        <v>0.1050658539103301</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="6"/>
+        <v>2.4541772743993075E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>7667</v>
+      </c>
+      <c r="B9" s="1">
+        <v>252.37459999999999</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-95.40746</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4074600000000004</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7667</v>
+      </c>
+      <c r="F9" s="1">
+        <v>252.37459999999999</v>
+      </c>
+      <c r="G9" s="1">
+        <v>-92.986310000000003</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>2.9863100000000031</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>4.9112349999999978</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="3"/>
+        <v>252.37459999999999</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="4"/>
+        <v>8.5717221089183671E-2</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="6"/>
+        <v>2.1128519592330332E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>8907</v>
+      </c>
+      <c r="B10" s="1">
+        <v>293.71199999999999</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-94.316869999999994</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3168699999999944</v>
+      </c>
+      <c r="E10" s="1">
+        <v>8907</v>
+      </c>
+      <c r="F10" s="1">
+        <v>293.71199999999999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-92.086060000000003</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>2.0860600000000034</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>3.9158149999999949</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="3"/>
+        <v>293.71199999999999</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="4"/>
+        <v>6.8343864648981664E-2</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="6"/>
+        <v>1.9467489743207275E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>10184</v>
+      </c>
+      <c r="B11" s="1">
+        <v>336.28280000000001</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-93.375200000000007</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3752000000000066</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10184</v>
+      </c>
+      <c r="F11" s="1">
+        <v>336.28280000000001</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-91.384110000000007</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.3841100000000068</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>3.0940050000000028</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="3"/>
+        <v>336.28280000000001</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="4"/>
+        <v>5.4000574323167204E-2</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="6"/>
+        <v>1.7375538101766945E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>11422</v>
+      </c>
+      <c r="B12" s="1">
+        <v>377.55349999999999</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-92.59836</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5983599999999996</v>
+      </c>
+      <c r="E12" s="1">
+        <v>11422</v>
+      </c>
+      <c r="F12" s="1">
+        <v>377.55349999999999</v>
+      </c>
+      <c r="G12" s="1">
+        <v>-90.943560000000005</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.94356000000000506</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>2.4853099999999984</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="3"/>
+        <v>377.55349999999999</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="4"/>
+        <v>4.3376842432740245E-2</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4440854231001036E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>12700</v>
+      </c>
+      <c r="B13" s="1">
+        <v>420.15769999999998</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-91.971800000000002</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9718000000000018</v>
+      </c>
+      <c r="E13" s="1">
+        <v>12700</v>
+      </c>
+      <c r="F13" s="1">
+        <v>420.15769999999998</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-90.457800000000006</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.45780000000000598</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>1.9291499999999999</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="3"/>
+        <v>420.15769999999998</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="4"/>
+        <v>3.3670019264848604E-2</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="6"/>
+        <v>1.3212142437597038E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>13938</v>
+      </c>
+      <c r="B14" s="1">
+        <v>461.42840000000001</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-91.792360000000002</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7923600000000022</v>
+      </c>
+      <c r="E14" s="1">
+        <v>13939</v>
+      </c>
+      <c r="F14" s="1">
+        <v>461.46170000000001</v>
+      </c>
+      <c r="G14" s="1">
+        <v>-90.169780000000003</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.16978000000000293</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>1.6954199999999986</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="3"/>
+        <v>461.46170000000001</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="4"/>
+        <v>2.9590661204162236E-2</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="6"/>
+        <v>1.415968168850479E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>15214</v>
+      </c>
+      <c r="B15" s="1">
+        <v>503.96589999999998</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-91.420599999999993</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4205999999999932</v>
+      </c>
+      <c r="E15" s="1">
+        <v>15214</v>
+      </c>
+      <c r="F15" s="1">
+        <v>503.96589999999998</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-89.74691</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.25309000000000026</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>1.2981049999999925</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="3"/>
+        <v>503.96589999999998</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="4"/>
+        <v>2.2656206286600859E-2</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4605700578851889E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>16451</v>
+      </c>
+      <c r="B16" s="1">
+        <v>545.20320000000004</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-90.902969999999996</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.90296999999999628</v>
+      </c>
+      <c r="E16" s="1">
+        <v>16451</v>
+      </c>
+      <c r="F16" s="1">
+        <v>545.20320000000004</v>
+      </c>
+      <c r="G16" s="1">
+        <v>-89.734080000000006</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.26591999999999416</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>1.0328749999999971</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="3"/>
+        <v>545.20320000000004</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="4"/>
+        <v>1.8027069511536382E-2</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="6"/>
+        <v>1.0200489546818176E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>17727</v>
+      </c>
+      <c r="B17" s="1">
+        <v>587.74069999999995</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-90.853809999999996</v>
+      </c>
+      <c r="D17" s="1">
+        <f>-90-C17</f>
+        <v>0.85380999999999574</v>
+      </c>
+      <c r="E17" s="1">
+        <v>17727</v>
+      </c>
+      <c r="F17" s="1">
+        <v>587.74069999999995</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-89.643129999999999</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.35687000000000069</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>0.96281999999999357</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="3"/>
+        <v>587.74069999999995</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="4"/>
+        <v>1.6804379104051692E-2</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="6"/>
+        <v>1.0565176094022443E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
@@ -2614,7 +4447,8 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
@@ -2628,28 +4462,939 @@
         <v>24</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
       <c r="B26" s="1">
-        <v>420</v>
+        <v>134</v>
       </c>
       <c r="C26" s="1">
-        <v>586</v>
-      </c>
-      <c r="D26" s="1">
+        <v>324</v>
+      </c>
+      <c r="D26" s="2">
         <f>(C26-B26)+1</f>
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="E26" s="1">
         <f>D26/5</f>
-        <v>33.4</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="F26" s="1">
         <f>E26*(1/30)</f>
-        <v>1.1133333333333333</v>
-      </c>
+        <v>1.2733333333333334</v>
+      </c>
+      <c r="G26">
+        <f>F26/(2*PI())</f>
+        <v>0.20265729420368009</v>
+      </c>
+      <c r="H26">
+        <f>(G26*G26)*9.81</f>
+        <v>0.40289649294971769</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC6832F-4A49-43A3-A70E-4DD1B53AB38B}">
+  <dimension ref="A1:O26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>428</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-117.1588</v>
+      </c>
+      <c r="D3" s="1">
+        <f>-90-C3</f>
+        <v>27.158799999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>428</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-108.044</v>
+      </c>
+      <c r="H3" s="1">
+        <f>-90-G3</f>
+        <v>18.043999999999997</v>
+      </c>
+      <c r="I3" s="1">
+        <v>447.5437</v>
+      </c>
+      <c r="J3" s="1">
+        <v>-87.924499999999995</v>
+      </c>
+      <c r="K3" s="2">
+        <f>(D3+H3)/2+$J$6</f>
+        <v>22.134104999999998</v>
+      </c>
+      <c r="L3" s="2">
+        <f>F3</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <f>RADIANS(K3)</f>
+        <v>0.38631300923213946</v>
+      </c>
+      <c r="N3" s="2">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O3" s="2">
+        <f>RADIANS((D3-H3)/2)</f>
+        <v>7.954163533038959E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>1697</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42.304119999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-109.773</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:D17" si="0">-90-C4</f>
+        <v>19.772999999999996</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1697</v>
+      </c>
+      <c r="F4" s="1">
+        <v>42.304119999999998</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-102.94799999999999</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H17" si="1">-90-G4</f>
+        <v>12.947999999999993</v>
+      </c>
+      <c r="I4" s="1">
+        <v>448.1438</v>
+      </c>
+      <c r="J4" s="1">
+        <v>-93.010090000000005</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" ref="K4:K17" si="2">(D4+H4)/2+$J$6</f>
+        <v>15.893204999999995</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" ref="L4:L17" si="3">F4</f>
+        <v>42.304119999999998</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" ref="M4:M17" si="4">RADIANS(K4)</f>
+        <v>0.2773887559444253</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N17" si="5">1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" ref="O4:O17" si="6">RADIANS((D4-H4)/2)</f>
+        <v>5.9559360724306523E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>2962</v>
+      </c>
+      <c r="B5" s="1">
+        <v>84.474909999999994</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-105.7306</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>15.730599999999995</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2962</v>
+      </c>
+      <c r="F5" s="1">
+        <v>84.474909999999994</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-99.815119999999993</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="1"/>
+        <v>9.8151199999999932</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="2">
+        <f t="shared" si="2"/>
+        <v>12.305564999999994</v>
+      </c>
+      <c r="L5" s="2">
+        <f t="shared" si="3"/>
+        <v>84.474909999999994</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="4"/>
+        <v>0.21477262556817592</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" si="6"/>
+        <v>5.1622301417937104E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>4223</v>
+      </c>
+      <c r="B6" s="1">
+        <v>126.5123</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-102.3831</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>12.383099999999999</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4224</v>
+      </c>
+      <c r="F6" s="1">
+        <v>126.5457</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-97.471900000000005</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="1"/>
+        <v>7.4719000000000051</v>
+      </c>
+      <c r="I6" s="1">
+        <f>90+J3</f>
+        <v>2.0755000000000052</v>
+      </c>
+      <c r="J6" s="1">
+        <f>AVERAGE(I6:I7)</f>
+        <v>-0.46729500000000002</v>
+      </c>
+      <c r="K6" s="2">
+        <f t="shared" si="2"/>
+        <v>9.460205000000002</v>
+      </c>
+      <c r="L6" s="2">
+        <f t="shared" si="3"/>
+        <v>126.5457</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="4"/>
+        <v>0.16511172516363021</v>
+      </c>
+      <c r="N6" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="6"/>
+        <v>4.2858305111972701E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>5446</v>
+      </c>
+      <c r="B7" s="1">
+        <v>167.28299999999999</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-100.4234</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>10.423400000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5447</v>
+      </c>
+      <c r="F7" s="1">
+        <v>167.31630000000001</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-95.922309999999996</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="1"/>
+        <v>5.922309999999996</v>
+      </c>
+      <c r="I7" s="1">
+        <f>90+J4</f>
+        <v>-3.0100900000000053</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" si="2"/>
+        <v>7.7055599999999984</v>
+      </c>
+      <c r="L7" s="2">
+        <f t="shared" si="3"/>
+        <v>167.31630000000001</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="4"/>
+        <v>0.13448739270997423</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="6"/>
+        <v>3.9279420214295827E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>6707</v>
+      </c>
+      <c r="B8" s="1">
+        <v>209.32040000000001</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-98.765429999999995</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>8.7654299999999949</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6707</v>
+      </c>
+      <c r="F8" s="1">
+        <v>209.32040000000001</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-94.735590000000002</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>4.735590000000002</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="2"/>
+        <v>6.2832149999999984</v>
+      </c>
+      <c r="L8" s="2">
+        <f t="shared" si="3"/>
+        <v>209.32040000000001</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="4"/>
+        <v>0.10966278936069548</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="6"/>
+        <v>3.5166988164284083E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>7968</v>
+      </c>
+      <c r="B9" s="1">
+        <v>251.3579</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-97.213120000000004</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>7.2131200000000035</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7969</v>
+      </c>
+      <c r="F9" s="1">
+        <v>251.3912</v>
+      </c>
+      <c r="G9" s="1">
+        <v>-93.517719999999997</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5177199999999971</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="2"/>
+        <v>4.8981250000000003</v>
+      </c>
+      <c r="L9" s="2">
+        <f t="shared" si="3"/>
+        <v>251.3912</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="4"/>
+        <v>8.5488408424247264E-2</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="6"/>
+        <v>3.2248448589099282E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>9228</v>
+      </c>
+      <c r="B10" s="1">
+        <v>293.36200000000002</v>
+      </c>
+      <c r="C10" s="1">
+        <v>-95.464979999999997</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4649799999999971</v>
+      </c>
+      <c r="E10" s="1">
+        <v>9228</v>
+      </c>
+      <c r="F10" s="1">
+        <v>293.36200000000002</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-92.824299999999994</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8242999999999938</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="2"/>
+        <v>3.6773449999999954</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" si="3"/>
+        <v>293.36200000000002</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="4"/>
+        <v>6.4181777981750801E-2</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="6"/>
+        <v>2.3044280245781958E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>10487</v>
+      </c>
+      <c r="B11" s="1">
+        <v>335.33269999999999</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-94.918270000000007</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>4.9182700000000068</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10488</v>
+      </c>
+      <c r="F11" s="1">
+        <v>335.36610000000002</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-92.398790000000005</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3987900000000053</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="2"/>
+        <v>3.191235000000006</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="3"/>
+        <v>335.36610000000002</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="4"/>
+        <v>5.5697557954881349E-2</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="6"/>
+        <v>2.1986610719073381E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>11748</v>
+      </c>
+      <c r="B12" s="1">
+        <v>377.37020000000001</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-93.996679999999998</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>3.9966799999999978</v>
+      </c>
+      <c r="E12" s="1">
+        <v>11747</v>
+      </c>
+      <c r="F12" s="1">
+        <v>377.33679999999998</v>
+      </c>
+      <c r="G12" s="1">
+        <v>-91.846069999999997</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8460699999999974</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="2"/>
+        <v>2.4540799999999976</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="3"/>
+        <v>377.33679999999998</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="4"/>
+        <v>4.2831776107342401E-2</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="6"/>
+        <v>1.876761271315763E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>13006</v>
+      </c>
+      <c r="B13" s="1">
+        <v>419.30759999999998</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-93.678569999999993</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6785699999999935</v>
+      </c>
+      <c r="E13" s="1">
+        <v>13005</v>
+      </c>
+      <c r="F13" s="1">
+        <v>419.27429999999998</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-91.604179999999999</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6041799999999995</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1740799999999965</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="3"/>
+        <v>419.27429999999998</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="4"/>
+        <v>3.7944854201758256E-2</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="6"/>
+        <v>1.8102467735222533E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>14264</v>
+      </c>
+      <c r="B14" s="1">
+        <v>461.245</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-93.016909999999996</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>3.0169099999999958</v>
+      </c>
+      <c r="E14" s="1">
+        <v>14264</v>
+      </c>
+      <c r="F14" s="1">
+        <v>461.245</v>
+      </c>
+      <c r="G14" s="1">
+        <v>-91.262209999999996</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2622099999999961</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="2"/>
+        <v>1.6722649999999959</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" si="3"/>
+        <v>461.245</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="4"/>
+        <v>2.9186530215862903E-2</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="6"/>
+        <v>1.5312646192372248E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>15563</v>
+      </c>
+      <c r="B15" s="1">
+        <v>504.54930000000002</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-92.716530000000006</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7165300000000059</v>
+      </c>
+      <c r="E15" s="1">
+        <v>15563</v>
+      </c>
+      <c r="F15" s="1">
+        <v>504.54930000000002</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-90.846720000000005</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8467200000000048</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3143300000000053</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="3"/>
+        <v>504.54930000000002</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="4"/>
+        <v>2.2939385957737164E-2</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="6"/>
+        <v>1.6317170443357596E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>16819</v>
+      </c>
+      <c r="B16" s="1">
+        <v>546.41999999999996</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-92.314809999999994</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3148099999999943</v>
+      </c>
+      <c r="E16" s="1">
+        <v>16819</v>
+      </c>
+      <c r="F16" s="1">
+        <v>546.41999999999996</v>
+      </c>
+      <c r="G16" s="1">
+        <v>-90.652079999999998</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.65207999999999799</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="2"/>
+        <v>1.0161499999999961</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="3"/>
+        <v>546.41999999999996</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="4"/>
+        <v>1.7735163194140313E-2</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="6"/>
+        <v>1.4510056535842626E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>18077</v>
+      </c>
+      <c r="B17" s="1">
+        <v>588.35739999999998</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-92.166470000000004</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1664700000000039</v>
+      </c>
+      <c r="E17" s="1">
+        <v>18077</v>
+      </c>
+      <c r="F17" s="1">
+        <v>588.35739999999998</v>
+      </c>
+      <c r="G17" s="1">
+        <v>-90.409679999999994</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.40967999999999449</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="2"/>
+        <v>0.82077999999999918</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="3"/>
+        <v>588.35739999999998</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="4"/>
+        <v>1.4325313434519043E-2</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="6"/>
+        <v>1.5330884883055673E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
+      <c r="B26" s="5">
+        <v>468</v>
+      </c>
+      <c r="C26" s="5">
+        <v>667</v>
+      </c>
+      <c r="D26" s="5">
+        <f>(C26-B26)+1</f>
+        <v>200</v>
+      </c>
+      <c r="E26" s="5">
+        <f>D26/5</f>
+        <v>40</v>
+      </c>
+      <c r="F26" s="5">
+        <f>E26*(1/30)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="G26" s="5">
+        <f>F26/(2*PI())</f>
+        <v>0.21220659078919377</v>
+      </c>
+      <c r="H26" s="5">
+        <f>(G26*G26)*9.81</f>
+        <v>0.44176036068059266</v>
+      </c>
+      <c r="I26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
all but len 2 done
</commit_message>
<xml_diff>
--- a/plotting/raw_retake.xlsx
+++ b/plotting/raw_retake.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\GitHub\Togohogo1-Archive\phy180-pendulum-report\plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C646273-5516-45C1-AA46-F385A65B6C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6107E8B8-6B24-4226-A4CA-EA6295C01DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="local" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="len7" sheetId="5" r:id="rId5"/>
     <sheet name="len8" sheetId="6" r:id="rId6"/>
     <sheet name="len9" sheetId="7" r:id="rId7"/>
+    <sheet name="len6" sheetId="8" r:id="rId8"/>
+    <sheet name="len2" sheetId="9" r:id="rId9"/>
+    <sheet name="len4" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -76,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="33">
   <si>
     <t>t</t>
   </si>
@@ -534,12 +537,12 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -559,7 +562,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.3</v>
       </c>
@@ -583,7 +586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4.5999999999999996</v>
       </c>
@@ -604,7 +607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4.5</v>
       </c>
@@ -629,7 +632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4.5</v>
       </c>
@@ -650,7 +653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4.5</v>
       </c>
@@ -675,7 +678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4.5</v>
       </c>
@@ -696,7 +699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4.5</v>
       </c>
@@ -720,7 +723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4.5</v>
       </c>
@@ -741,7 +744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4.5</v>
       </c>
@@ -764,6 +767,87 @@
       </c>
       <c r="G10">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D9068D-7589-4BE7-ABA6-164710920B48}">
+  <dimension ref="A24:H26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="5">
+        <v>67</v>
+      </c>
+      <c r="C26" s="5">
+        <v>217</v>
+      </c>
+      <c r="D26" s="5">
+        <f>(C26-B26)+1</f>
+        <v>151</v>
+      </c>
+      <c r="E26" s="5">
+        <f>D26/5</f>
+        <v>30.2</v>
+      </c>
+      <c r="F26" s="5">
+        <f>E26*(1/30)</f>
+        <v>1.0066666666666666</v>
+      </c>
+      <c r="G26" s="5">
+        <f>F26/(2*PI())</f>
+        <v>0.16021597604584131</v>
+      </c>
+      <c r="H26" s="5">
+        <f>(G26*G26)*9.81</f>
+        <v>0.25181444959695487</v>
       </c>
     </row>
   </sheetData>
@@ -779,18 +863,18 @@
       <selection activeCell="M2" sqref="M2:P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -801,7 +885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -845,7 +929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>218</v>
       </c>
@@ -895,7 +979,7 @@
         <v>1.4351842439149345E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>668</v>
       </c>
@@ -945,7 +1029,7 @@
         <v>1.1623020153656276E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1116</v>
       </c>
@@ -995,7 +1079,7 @@
         <v>1.2941616403537989E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1564</v>
       </c>
@@ -1045,7 +1129,7 @@
         <v>1.4474015486788911E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2011</v>
       </c>
@@ -1096,7 +1180,7 @@
         <v>1.210734902108466E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2458</v>
       </c>
@@ -1147,7 +1231,7 @@
         <v>8.4583018874775408E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2924</v>
       </c>
@@ -1198,7 +1282,7 @@
         <v>1.0399020749232673E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3370</v>
       </c>
@@ -1245,7 +1329,7 @@
         <v>1.0561510902593208E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3815</v>
       </c>
@@ -1292,7 +1376,7 @@
         <v>1.202793654011901E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4260</v>
       </c>
@@ -1339,7 +1423,7 @@
         <v>1.0931957036329024E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4725</v>
       </c>
@@ -1386,7 +1470,7 @@
         <v>1.0450595228629105E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>5169</v>
       </c>
@@ -1433,7 +1517,7 @@
         <v>1.0450071629853465E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>5612</v>
       </c>
@@ -1480,7 +1564,7 @@
         <v>9.5215564677925378E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>6076</v>
       </c>
@@ -1527,7 +1611,7 @@
         <v>8.0088796050889633E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>6518</v>
       </c>
@@ -1574,7 +1658,7 @@
         <v>9.6359628002607445E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>6961</v>
       </c>
@@ -1621,7 +1705,7 @@
         <v>9.5386606944620547E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>7422</v>
       </c>
@@ -1668,7 +1752,7 @@
         <v>1.0139490289461083E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>7863</v>
       </c>
@@ -1715,7 +1799,7 @@
         <v>9.2080953341343186E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>8325</v>
       </c>
@@ -1762,7 +1846,7 @@
         <v>8.8325877455676001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>8765</v>
       </c>
@@ -1809,12 +1893,12 @@
         <v>9.4666658628172543E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>239</v>
       </c>
@@ -1834,7 +1918,7 @@
         <v>0.68666666666666676</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>19</v>
       </c>
@@ -1854,24 +1938,24 @@
       <selection activeCell="M2" sqref="M2:P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="1"/>
-    <col min="9" max="9" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.26953125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="9.1796875" style="1"/>
-    <col min="14" max="14" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="1" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1885,7 +1969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1926,7 +2010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>209</v>
       </c>
@@ -1979,7 +2063,7 @@
         <v>2.1314833489980835E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1152</v>
       </c>
@@ -2032,7 +2116,7 @@
         <v>1.5928747418326235E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2065</v>
       </c>
@@ -2082,7 +2166,7 @@
         <v>1.2749630185818565E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3003</v>
       </c>
@@ -2133,7 +2217,7 @@
         <v>1.0797479417462837E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3940</v>
       </c>
@@ -2184,7 +2268,7 @@
         <v>1.0824532020868778E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4848</v>
       </c>
@@ -2235,7 +2319,7 @@
         <v>1.6174489777007035E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5783</v>
       </c>
@@ -2282,7 +2366,7 @@
         <v>1.5263864239779023E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6718</v>
       </c>
@@ -2329,7 +2413,7 @@
         <v>1.4231676520149589E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7651</v>
       </c>
@@ -2376,7 +2460,7 @@
         <v>1.3859223257773962E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8585</v>
       </c>
@@ -2423,7 +2507,7 @@
         <v>1.4931379017274104E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9517</v>
       </c>
@@ -2470,7 +2554,7 @@
         <v>1.6320661101861575E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10450</v>
       </c>
@@ -2517,7 +2601,7 @@
         <v>1.3734606749181573E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>11382</v>
       </c>
@@ -2564,7 +2648,7 @@
         <v>1.6639358223275828E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>12313</v>
       </c>
@@ -2611,7 +2695,7 @@
         <v>1.1792578890487401E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13244</v>
       </c>
@@ -2658,12 +2742,12 @@
         <v>1.1403894066068282E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
@@ -2680,7 +2764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>1057</v>
       </c>
@@ -2713,23 +2797,23 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="1"/>
-    <col min="9" max="10" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.08984375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="8.7109375" style="1"/>
+    <col min="9" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2740,7 +2824,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2790,7 +2874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>387</v>
       </c>
@@ -2846,7 +2930,7 @@
         <v>4.2529310547971766E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1482</v>
       </c>
@@ -2902,7 +2986,7 @@
         <v>3.6655404950384926E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2540</v>
       </c>
@@ -2952,7 +3036,7 @@
         <v>3.0737866121498147E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3630</v>
       </c>
@@ -3003,7 +3087,7 @@
         <v>2.5806438319988158E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4719</v>
       </c>
@@ -3054,7 +3138,7 @@
         <v>2.0882777233649532E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5807</v>
       </c>
@@ -3105,7 +3189,7 @@
         <v>1.9980442010368395E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6860</v>
       </c>
@@ -3152,7 +3236,7 @@
         <v>1.6013832219360931E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7947</v>
       </c>
@@ -3199,7 +3283,7 @@
         <v>1.5342404056118648E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9033</v>
       </c>
@@ -3246,7 +3330,7 @@
         <v>1.1478681424516291E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10120</v>
       </c>
@@ -3293,7 +3377,7 @@
         <v>1.5474874546345149E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11204</v>
       </c>
@@ -3340,7 +3424,7 @@
         <v>1.5069696360494657E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12290</v>
       </c>
@@ -3387,7 +3471,7 @@
         <v>1.3727014566935343E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13375</v>
       </c>
@@ -3434,7 +3518,7 @@
         <v>1.0569452150689822E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14425</v>
       </c>
@@ -3481,7 +3565,7 @@
         <v>1.2487830798019406E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15511</v>
       </c>
@@ -3528,7 +3612,7 @@
         <v>1.1400927006339942E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16199</v>
       </c>
@@ -3575,12 +3659,12 @@
         <v>1.2742736135273231E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
@@ -3597,7 +3681,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>420</v>
       </c>
@@ -3630,19 +3714,19 @@
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -3653,7 +3737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3700,7 +3784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>96</v>
       </c>
@@ -3754,7 +3838,7 @@
         <v>6.2477551233641057E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1344</v>
       </c>
@@ -3808,7 +3892,7 @@
         <v>5.1164327022213768E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2627</v>
       </c>
@@ -3859,7 +3943,7 @@
         <v>4.2736917462496533E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3869</v>
       </c>
@@ -3911,7 +3995,7 @@
         <v>3.5241077391031321E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5149</v>
       </c>
@@ -3963,7 +4047,7 @@
         <v>2.9592755599264674E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6390</v>
       </c>
@@ -4015,7 +4099,7 @@
         <v>2.4541772743993075E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7667</v>
       </c>
@@ -4063,7 +4147,7 @@
         <v>2.1128519592330332E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8907</v>
       </c>
@@ -4111,7 +4195,7 @@
         <v>1.9467489743207275E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10184</v>
       </c>
@@ -4159,7 +4243,7 @@
         <v>1.7375538101766945E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11422</v>
       </c>
@@ -4207,7 +4291,7 @@
         <v>1.4440854231001036E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12700</v>
       </c>
@@ -4255,7 +4339,7 @@
         <v>1.3212142437597038E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13938</v>
       </c>
@@ -4303,7 +4387,7 @@
         <v>1.415968168850479E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>15214</v>
       </c>
@@ -4351,7 +4435,7 @@
         <v>1.4605700578851889E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>16451</v>
       </c>
@@ -4399,7 +4483,7 @@
         <v>1.0200489546818176E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>17727</v>
       </c>
@@ -4447,7 +4531,7 @@
         <v>1.0565176094022443E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -4457,7 +4541,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -4481,7 +4565,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1">
         <v>134</v>
@@ -4523,21 +4607,21 @@
       <selection activeCell="A24" sqref="A24:H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -4548,7 +4632,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4595,7 +4679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>428</v>
       </c>
@@ -4649,7 +4733,7 @@
         <v>7.954163533038959E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1697</v>
       </c>
@@ -4703,7 +4787,7 @@
         <v>5.9559360724306523E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2962</v>
       </c>
@@ -4754,7 +4838,7 @@
         <v>5.1622301417937104E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4223</v>
       </c>
@@ -4810,7 +4894,7 @@
         <v>4.2858305111972701E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5446</v>
       </c>
@@ -4862,7 +4946,7 @@
         <v>3.9279420214295827E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6707</v>
       </c>
@@ -4910,7 +4994,7 @@
         <v>3.5166988164284083E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7968</v>
       </c>
@@ -4958,7 +5042,7 @@
         <v>3.2248448589099282E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9228</v>
       </c>
@@ -5006,7 +5090,7 @@
         <v>2.3044280245781958E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10487</v>
       </c>
@@ -5054,7 +5138,7 @@
         <v>2.1986610719073381E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11748</v>
       </c>
@@ -5102,7 +5186,7 @@
         <v>1.876761271315763E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>13006</v>
       </c>
@@ -5150,7 +5234,7 @@
         <v>1.8102467735222533E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>14264</v>
       </c>
@@ -5198,7 +5282,7 @@
         <v>1.5312646192372248E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>15563</v>
       </c>
@@ -5246,7 +5330,7 @@
         <v>1.6317170443357596E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>16819</v>
       </c>
@@ -5294,7 +5378,7 @@
         <v>1.4510056535842626E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>18077</v>
       </c>
@@ -5342,7 +5426,7 @@
         <v>1.5330884883055673E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -5352,7 +5436,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -5376,7 +5460,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="5">
         <v>468</v>
@@ -5415,23 +5499,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8740C19F-6777-4FB3-9718-68300DD6568C}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -5443,7 +5527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -5490,7 +5574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>355</v>
       </c>
@@ -5530,24 +5614,24 @@
         <f>(D3+H3)/2-$J$8</f>
         <v>21.339029999999987</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="2">
         <f>F3</f>
         <v>0</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="2">
         <f>RADIANS(L3)</f>
         <v>0.37243633268184534</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="2">
         <f>1/30</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="2">
         <f>RADIANS((D3-H3)/2)</f>
         <v>8.0254602329829255E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1577</v>
       </c>
@@ -5587,24 +5671,24 @@
         <f t="shared" ref="L4:L17" si="2">(D4+H4)/2-$J$8</f>
         <v>15.706379999999982</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="2">
         <f t="shared" ref="M4:M17" si="3">F4</f>
         <v>40.695639999999997</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="2">
         <f t="shared" ref="N4:N17" si="4">RADIANS(L4)</f>
         <v>0.27412804456938666</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="2">
         <f t="shared" ref="O4:O17" si="5">1/30</f>
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="2">
         <f t="shared" ref="P4:P17" si="6">RADIANS((D4-H4)/2)</f>
         <v>6.3343234542630217E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2796</v>
       </c>
@@ -5638,24 +5722,24 @@
         <f t="shared" si="2"/>
         <v>11.828274999999984</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="2">
         <f t="shared" si="3"/>
         <v>81.33296</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="2">
         <f t="shared" si="4"/>
         <v>0.20644234358133201</v>
       </c>
-      <c r="O5">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P5">
+      <c r="O5" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P5" s="2">
         <f t="shared" si="6"/>
         <v>4.8082162829654398E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4013</v>
       </c>
@@ -5692,24 +5776,24 @@
         <f t="shared" si="2"/>
         <v>9.1652799999999885</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="2">
         <f t="shared" si="3"/>
         <v>121.93689999999999</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="2">
         <f t="shared" si="4"/>
         <v>0.15996431286718568</v>
       </c>
-      <c r="O6">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P6">
+      <c r="O6" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P6" s="2">
         <f t="shared" si="6"/>
         <v>3.7370989943702672E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5228</v>
       </c>
@@ -5746,24 +5830,24 @@
         <f t="shared" si="2"/>
         <v>7.3317049999999853</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="2">
         <f t="shared" si="3"/>
         <v>162.4742</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="2">
         <f t="shared" si="4"/>
         <v>0.12796239203493059</v>
       </c>
-      <c r="O7">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P7">
+      <c r="O7" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P7" s="2">
         <f t="shared" si="6"/>
         <v>2.8463789372612069E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6444</v>
       </c>
@@ -5800,24 +5884,24 @@
         <f t="shared" si="2"/>
         <v>5.8449949999999902</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="2">
         <f t="shared" si="3"/>
         <v>202.97819999999999</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="2">
         <f t="shared" si="4"/>
         <v>0.10201440751260579</v>
       </c>
-      <c r="O8">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P8">
+      <c r="O8" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P8" s="2">
         <f t="shared" si="6"/>
         <v>2.2296668460690124E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7658</v>
       </c>
@@ -5853,24 +5937,24 @@
         <f t="shared" si="2"/>
         <v>4.6249499999999912</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="2">
         <f t="shared" si="3"/>
         <v>243.44880000000001</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="2">
         <f t="shared" si="4"/>
         <v>8.0720605240111598E-2</v>
       </c>
-      <c r="O9">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P9">
+      <c r="O9" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P9" s="2">
         <f t="shared" si="6"/>
         <v>2.0744808956279365E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8874</v>
       </c>
@@ -5904,24 +5988,24 @@
         <f t="shared" si="2"/>
         <v>3.616359999999986</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="2">
         <f t="shared" si="3"/>
         <v>283.98610000000002</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="2">
         <f t="shared" si="4"/>
         <v>6.3117388937421887E-2</v>
       </c>
-      <c r="O10">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P10">
+      <c r="O10" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P10" s="2">
         <f t="shared" si="6"/>
         <v>1.6014792150449587E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10087</v>
       </c>
@@ -5955,24 +6039,24 @@
         <f t="shared" si="2"/>
         <v>3.1248899999999935</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="2">
         <f t="shared" si="3"/>
         <v>324.42340000000002</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="2">
         <f t="shared" si="4"/>
         <v>5.4539619262645493E-2</v>
       </c>
-      <c r="O11">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P11">
+      <c r="O11" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P11" s="2">
         <f t="shared" si="6"/>
         <v>1.5708486866724582E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11302</v>
       </c>
@@ -6006,24 +6090,24 @@
         <f t="shared" si="2"/>
         <v>2.6685249999999883</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="2">
         <f t="shared" si="3"/>
         <v>364.9273</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="2">
         <f t="shared" si="4"/>
         <v>4.6574547421781479E-2</v>
       </c>
-      <c r="O12">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P12">
+      <c r="O12" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P12" s="2">
         <f t="shared" si="6"/>
         <v>1.3673694758286982E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12515</v>
       </c>
@@ -6057,24 +6141,24 @@
         <f t="shared" si="2"/>
         <v>2.2710399999999851</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="2">
         <f t="shared" si="3"/>
         <v>405.3646</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="2">
         <f t="shared" si="4"/>
         <v>3.9637125444491758E-2</v>
       </c>
-      <c r="O13">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P13">
+      <c r="O13" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P13" s="2">
         <f t="shared" si="6"/>
         <v>1.5054337463077069E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13728</v>
       </c>
@@ -6108,24 +6192,24 @@
         <f t="shared" si="2"/>
         <v>1.7579749999999876</v>
       </c>
-      <c r="M14" s="1">
+      <c r="M14" s="2">
         <f t="shared" si="3"/>
         <v>445.80189999999999</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="2">
         <f t="shared" si="4"/>
         <v>3.06824519177471E-2</v>
       </c>
-      <c r="O14">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P14">
+      <c r="O14" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P14" s="2">
         <f t="shared" si="6"/>
         <v>1.2523697314147987E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14942</v>
       </c>
@@ -6159,24 +6243,24 @@
         <f t="shared" si="2"/>
         <v>1.5530399999999887</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15" s="2">
         <f t="shared" si="3"/>
         <v>486.27249999999998</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="2">
         <f t="shared" si="4"/>
         <v>2.7105661415172538E-2</v>
       </c>
-      <c r="O15">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P15">
+      <c r="O15" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P15" s="2">
         <f t="shared" si="6"/>
         <v>1.2716294397105556E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>16156</v>
       </c>
@@ -6210,24 +6294,24 @@
         <f t="shared" si="2"/>
         <v>1.4297149999999874</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="2">
         <f t="shared" si="3"/>
         <v>526.74310000000003</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="2">
         <f t="shared" si="4"/>
         <v>2.4953234115150508E-2</v>
       </c>
-      <c r="O16">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P16">
+      <c r="O16" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P16" s="2">
         <f t="shared" si="6"/>
         <v>1.5177819507655675E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>17368</v>
       </c>
@@ -6261,24 +6345,24 @@
         <f t="shared" si="2"/>
         <v>1.051774999999985</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17" s="2">
         <f t="shared" si="3"/>
         <v>567.14710000000002</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="2">
         <f t="shared" si="4"/>
         <v>1.8356936740163098E-2</v>
       </c>
-      <c r="O17">
-        <f t="shared" si="5"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="P17">
+      <c r="O17" s="2">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P17" s="2">
         <f t="shared" si="6"/>
         <v>1.5675412877399333E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -6288,7 +6372,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -6312,7 +6396,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="5">
         <v>397</v>
@@ -6339,6 +6423,600 @@
       <c r="H26" s="5">
         <f>(G26*G26)*9.81</f>
         <v>0.49169032544651675</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A51BA204-7F14-4F48-A65D-48514DC4DF61}">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>412</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-113.6665</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>412</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-107.5153</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2">
+        <v>11934</v>
+      </c>
+      <c r="J3" s="2">
+        <v>384.10419999999999</v>
+      </c>
+      <c r="K3" s="2">
+        <v>-93.314999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1523</v>
+      </c>
+      <c r="B4" s="2">
+        <v>37.036830000000002</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-108.9589</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>1523</v>
+      </c>
+      <c r="F4" s="2">
+        <v>37.036830000000002</v>
+      </c>
+      <c r="G4" s="2">
+        <v>-103.8544</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2">
+        <v>11952</v>
+      </c>
+      <c r="J4" s="2">
+        <v>384.70420000000001</v>
+      </c>
+      <c r="K4" s="2">
+        <v>-87.058440000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2592</v>
+      </c>
+      <c r="B5" s="2">
+        <v>72.673770000000005</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-105.7448</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>2592</v>
+      </c>
+      <c r="F5" s="2">
+        <v>72.673770000000005</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-101.03019999999999</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>3660</v>
+      </c>
+      <c r="B6" s="2">
+        <v>108.27719999999999</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-102.9385</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>3660</v>
+      </c>
+      <c r="F6" s="2">
+        <v>108.27719999999999</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-98.936520000000002</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>4763</v>
+      </c>
+      <c r="B7" s="2">
+        <v>145.04750000000001</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-100.64960000000001</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>4763</v>
+      </c>
+      <c r="F7" s="2">
+        <v>145.04750000000001</v>
+      </c>
+      <c r="G7" s="2">
+        <v>-97.132570000000001</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>5829</v>
+      </c>
+      <c r="B8" s="2">
+        <v>180.58430000000001</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-98.979439999999997</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>5829</v>
+      </c>
+      <c r="F8" s="2">
+        <v>180.58430000000001</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-95.854910000000004</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>6930</v>
+      </c>
+      <c r="B9" s="2">
+        <v>217.28790000000001</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-97.435239999999993</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
+        <v>6930</v>
+      </c>
+      <c r="F9" s="2">
+        <v>217.28790000000001</v>
+      </c>
+      <c r="G9" s="2">
+        <v>-94.703000000000003</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>7995</v>
+      </c>
+      <c r="B10" s="2">
+        <v>252.79140000000001</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-96.221500000000006</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
+        <v>7995</v>
+      </c>
+      <c r="F10" s="2">
+        <v>252.79140000000001</v>
+      </c>
+      <c r="G10" s="2">
+        <v>-93.649900000000002</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9096</v>
+      </c>
+      <c r="B11" s="2">
+        <v>289.49489999999997</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-95.193489999999997</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
+        <v>9096</v>
+      </c>
+      <c r="F11" s="2">
+        <v>289.49489999999997</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-93.033010000000004</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10161</v>
+      </c>
+      <c r="B12" s="2">
+        <v>324.9984</v>
+      </c>
+      <c r="C12" s="2">
+        <v>-94.152150000000006</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
+        <v>10161</v>
+      </c>
+      <c r="F12" s="2">
+        <v>324.9984</v>
+      </c>
+      <c r="G12" s="2">
+        <v>-92.400109999999998</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>11260</v>
+      </c>
+      <c r="B13" s="2">
+        <v>361.63529999999997</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-93.816720000000004</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
+        <v>11260</v>
+      </c>
+      <c r="F13" s="2">
+        <v>361.63529999999997</v>
+      </c>
+      <c r="G13" s="2">
+        <v>-91.919759999999997</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>12325</v>
+      </c>
+      <c r="B14" s="2">
+        <v>397.1388</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-93.406440000000003</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
+        <v>12325</v>
+      </c>
+      <c r="F14" s="2">
+        <v>397.1388</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-91.426119999999997</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>13424</v>
+      </c>
+      <c r="B15" s="2">
+        <v>433.77569999999997</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-92.720460000000003</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
+        <v>13424</v>
+      </c>
+      <c r="F15" s="2">
+        <v>433.77569999999997</v>
+      </c>
+      <c r="G15" s="2">
+        <v>-91.133080000000007</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>14487</v>
+      </c>
+      <c r="B16" s="2">
+        <v>469.21249999999998</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-92.444590000000005</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2">
+        <v>14487</v>
+      </c>
+      <c r="F16" s="2">
+        <v>469.21249999999998</v>
+      </c>
+      <c r="G16" s="2">
+        <v>-90.809979999999996</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>15587</v>
+      </c>
+      <c r="B17" s="2">
+        <v>505.8827</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-92.127300000000005</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2">
+        <v>15587</v>
+      </c>
+      <c r="F17" s="2">
+        <v>505.8827</v>
+      </c>
+      <c r="G17" s="2">
+        <v>-90.555160000000001</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="5">
+        <v>452</v>
+      </c>
+      <c r="C26" s="5">
+        <v>630</v>
+      </c>
+      <c r="D26" s="5">
+        <f>(C26-B26)+1</f>
+        <v>179</v>
+      </c>
+      <c r="E26" s="5">
+        <f>D26/5</f>
+        <v>35.799999999999997</v>
+      </c>
+      <c r="F26" s="5">
+        <f>E26*(1/30)</f>
+        <v>1.1933333333333331</v>
+      </c>
+      <c r="G26" s="5">
+        <f>F26/(2*PI())</f>
+        <v>0.1899248987563284</v>
+      </c>
+      <c r="H26" s="5">
+        <f>(G26*G26)*9.81</f>
+        <v>0.35386109291417167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EB071B9-253B-4AAB-95CA-D7EC2A010F92}">
+  <dimension ref="A24:H26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="5">
+        <v>244</v>
+      </c>
+      <c r="C26" s="5">
+        <v>369</v>
+      </c>
+      <c r="D26" s="5">
+        <f>(C26-B26)+1</f>
+        <v>126</v>
+      </c>
+      <c r="E26" s="5">
+        <f>D26/5</f>
+        <v>25.2</v>
+      </c>
+      <c r="F26" s="5">
+        <f>E26*(1/30)</f>
+        <v>0.84</v>
+      </c>
+      <c r="G26" s="5">
+        <f>F26/(2*PI())</f>
+        <v>0.13369015219719207</v>
+      </c>
+      <c r="H26" s="5">
+        <f>(G26*G26)*9.81</f>
+        <v>0.17533468715412723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new lengths leading to more scuffed q factors
</commit_message>
<xml_diff>
--- a/plotting/raw_retake.xlsx
+++ b/plotting/raw_retake.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\GitHub\Togohogo1-Archive\phy180-pendulum-report\plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6107E8B8-6B24-4226-A4CA-EA6295C01DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED6FAC6-7972-4D5E-B7A1-B56F2E5D8A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="local" sheetId="2" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="33">
   <si>
     <t>t</t>
   </si>
@@ -537,7 +537,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,18 +776,923 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D9068D-7589-4BE7-ABA6-164710920B48}">
-  <dimension ref="A24:H26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-110.637</v>
+      </c>
+      <c r="D3" s="2">
+        <f>-90-C3</f>
+        <v>20.637</v>
+      </c>
+      <c r="E3" s="2">
+        <v>35</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-105.9151</v>
+      </c>
+      <c r="H3" s="2">
+        <f>-90-G3</f>
+        <v>15.915099999999995</v>
+      </c>
+      <c r="I3" s="2">
+        <v>7998</v>
+      </c>
+      <c r="J3" s="2">
+        <v>265.44260000000003</v>
+      </c>
+      <c r="K3" s="2">
+        <v>-94.269499999999994</v>
+      </c>
+      <c r="L3">
+        <f>(D3+H3)/2+$J$8</f>
+        <v>18.514720000000011</v>
+      </c>
+      <c r="M3" s="2">
+        <f>F3</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f>RADIANS(L3)</f>
+        <v>0.32314282408484474</v>
+      </c>
+      <c r="O3">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P3">
+        <f>RADIANS((D3-H3)/2)</f>
+        <v>4.1206350974960171E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1055</v>
+      </c>
+      <c r="B4" s="2">
+        <v>33.986640000000001</v>
+      </c>
+      <c r="C4" s="2">
+        <v>-107.92489999999999</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D18" si="0">-90-C4</f>
+        <v>17.924899999999994</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1055</v>
+      </c>
+      <c r="F4" s="2">
+        <v>33.986640000000001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>-103.49209999999999</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H18" si="1">-90-G4</f>
+        <v>13.492099999999994</v>
+      </c>
+      <c r="I4" s="2">
+        <v>8014</v>
+      </c>
+      <c r="J4" s="2">
+        <v>265.976</v>
+      </c>
+      <c r="K4" s="2">
+        <v>-85.491829999999993</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L18" si="2">(D4+H4)/2+$J$8</f>
+        <v>15.947170000000007</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" ref="M4:M18" si="3">F4</f>
+        <v>33.986640000000001</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N18" si="4">RADIANS(L4)</f>
+        <v>0.27833062287526422</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O18" si="5">1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P18" si="6">RADIANS((D4-H4)/2)</f>
+        <v>3.868347754120232E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2101</v>
+      </c>
+      <c r="B5" s="2">
+        <v>68.856719999999996</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-104.6583</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>14.658299999999997</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2101</v>
+      </c>
+      <c r="F5" s="2">
+        <v>68.856719999999996</v>
+      </c>
+      <c r="G5" s="2">
+        <v>-100.8502</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="1"/>
+        <v>10.850200000000001</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>12.992920000000012</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="3"/>
+        <v>68.856719999999996</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="4"/>
+        <v>0.22676923344822186</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="6"/>
+        <v>3.3231941622597995E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>3116</v>
+      </c>
+      <c r="B6" s="2">
+        <v>102.6934</v>
+      </c>
+      <c r="C6" s="2">
+        <v>-102.0809</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>12.0809</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3116</v>
+      </c>
+      <c r="F6" s="2">
+        <v>102.6934</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-98.566209999999998</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="1"/>
+        <v>8.5662099999999981</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
+        <f>-90-K3</f>
+        <v>4.2694999999999936</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>10.562225000000012</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="3"/>
+        <v>102.6934</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>0.1843456025864583</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="6"/>
+        <v>3.0671456343459764E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>4159</v>
+      </c>
+      <c r="B7" s="2">
+        <v>137.46340000000001</v>
+      </c>
+      <c r="C7" s="2">
+        <v>-99.880510000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>9.880510000000001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4159</v>
+      </c>
+      <c r="F7" s="2">
+        <v>137.46340000000001</v>
+      </c>
+      <c r="G7" s="2">
+        <v>-96.717799999999997</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="1"/>
+        <v>6.7177999999999969</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2">
+        <f>90+K4</f>
+        <v>4.5081700000000069</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>8.5378250000000122</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="3"/>
+        <v>137.46340000000001</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>0.14901315720908509</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="6"/>
+        <v>2.7599851392874967E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>5172</v>
+      </c>
+      <c r="B8" s="2">
+        <v>171.23339999999999</v>
+      </c>
+      <c r="C8" s="2">
+        <v>-98.084490000000002</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>8.0844900000000024</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5172</v>
+      </c>
+      <c r="F8" s="2">
+        <v>171.23339999999999</v>
+      </c>
+      <c r="G8" s="2">
+        <v>-95.404049999999998</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>5.404049999999998</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2">
+        <f>J7-J6</f>
+        <v>0.23867000000001326</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>6.9829400000000135</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="3"/>
+        <v>171.23339999999999</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>0.12187529446921307</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="6"/>
+        <v>2.339125170107844E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>6214</v>
+      </c>
+      <c r="B9" s="2">
+        <v>205.9701</v>
+      </c>
+      <c r="C9" s="2">
+        <v>-96.520340000000004</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>6.5203400000000045</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6214</v>
+      </c>
+      <c r="F9" s="2">
+        <v>205.9701</v>
+      </c>
+      <c r="G9" s="2">
+        <v>-94.091089999999994</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>4.0910899999999941</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>5.5443850000000126</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="3"/>
+        <v>205.9701</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>9.6767773248186029E-2</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>2.1199205427036214E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>7226</v>
+      </c>
+      <c r="B10" s="2">
+        <v>239.70670000000001</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-95.235789999999994</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>5.2357899999999944</v>
+      </c>
+      <c r="E10" s="2">
+        <v>7227</v>
+      </c>
+      <c r="F10" s="2">
+        <v>239.74010000000001</v>
+      </c>
+      <c r="G10" s="2">
+        <v>-93.031819999999996</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>3.0318199999999962</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>4.3724750000000085</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="3"/>
+        <v>239.74010000000001</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>7.6314085211139207E-2</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="6"/>
+        <v>1.9233266557589696E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>8267</v>
+      </c>
+      <c r="B11" s="2">
+        <v>274.4101</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-94.146960000000007</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>4.1469600000000071</v>
+      </c>
+      <c r="E11" s="2">
+        <v>8267</v>
+      </c>
+      <c r="F11" s="2">
+        <v>274.4101</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-92.056619999999995</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0566199999999952</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>3.3404600000000144</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="3"/>
+        <v>274.4101</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>5.8302025531170032E-2</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="6"/>
+        <v>1.8241657743069236E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>9278</v>
+      </c>
+      <c r="B12" s="2">
+        <v>308.11340000000001</v>
+      </c>
+      <c r="C12" s="2">
+        <v>-93.317300000000003</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>3.317300000000003</v>
+      </c>
+      <c r="E12" s="2">
+        <v>9278</v>
+      </c>
+      <c r="F12" s="2">
+        <v>308.11340000000001</v>
+      </c>
+      <c r="G12" s="2">
+        <v>-91.321780000000004</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>1.321780000000004</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>2.5582100000000167</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="3"/>
+        <v>308.11340000000001</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>4.4649187457444429E-2</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="6"/>
+        <v>1.7414197144698614E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>10318</v>
+      </c>
+      <c r="B13" s="2">
+        <v>342.7835</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-92.737110000000001</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>2.7371100000000013</v>
+      </c>
+      <c r="E13" s="2">
+        <v>10318</v>
+      </c>
+      <c r="F13" s="2">
+        <v>342.7835</v>
+      </c>
+      <c r="G13" s="2">
+        <v>-90.770759999999996</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.77075999999999567</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>1.9926050000000117</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="3"/>
+        <v>342.7835</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>3.4777517941701815E-2</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="6"/>
+        <v>1.7159640873295297E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>11357</v>
+      </c>
+      <c r="B14" s="2">
+        <v>377.42020000000002</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-92.196719999999999</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>2.1967199999999991</v>
+      </c>
+      <c r="E14" s="2">
+        <v>11357</v>
+      </c>
+      <c r="F14" s="2">
+        <v>377.42020000000002</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-90.395489999999995</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.39548999999999523</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>1.5347750000000104</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="3"/>
+        <v>377.42020000000002</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="4"/>
+        <v>2.6786877027296152E-2</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="6"/>
+        <v>1.5718697042848766E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>12366</v>
+      </c>
+      <c r="B15" s="2">
+        <v>411.05680000000001</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-91.709280000000007</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7092800000000068</v>
+      </c>
+      <c r="E15" s="2">
+        <v>12366</v>
+      </c>
+      <c r="F15" s="2">
+        <v>411.05680000000001</v>
+      </c>
+      <c r="G15" s="2">
+        <v>-90.141019999999997</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.14101999999999748</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>1.1638200000000154</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="3"/>
+        <v>411.05680000000001</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>2.0312490900560674E-2</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="6"/>
+        <v>1.3685650263663217E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>13405</v>
+      </c>
+      <c r="B16" s="2">
+        <v>445.69349999999997</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-91.583629999999999</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5836299999999994</v>
+      </c>
+      <c r="E16" s="2">
+        <v>13405</v>
+      </c>
+      <c r="F16" s="2">
+        <v>445.69349999999997</v>
+      </c>
+      <c r="G16" s="2">
+        <v>-90.134309999999999</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13430999999999926</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>1.0976400000000126</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="3"/>
+        <v>445.69349999999997</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>1.9157432001590778E-2</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="6"/>
+        <v>1.2647702957502109E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>14443</v>
+      </c>
+      <c r="B17" s="2">
+        <v>480.29689999999999</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-91.15231</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1523099999999999</v>
+      </c>
+      <c r="E17" s="2">
+        <v>14444</v>
+      </c>
+      <c r="F17" s="2">
+        <v>480.33019999999999</v>
+      </c>
+      <c r="G17" s="2">
+        <v>-89.993629999999996</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>-6.3700000000039836E-3</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>0.81164000000001124</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="3"/>
+        <v>480.33019999999999</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="4"/>
+        <v>1.4165790340886972E-2</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="6"/>
+        <v>1.0111390488503983E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>15419</v>
+      </c>
+      <c r="B18" s="2">
+        <v>512.83339999999998</v>
+      </c>
+      <c r="C18" s="2">
+        <v>-90.81926</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.81925999999999988</v>
+      </c>
+      <c r="E18" s="2">
+        <v>15419</v>
+      </c>
+      <c r="F18" s="2">
+        <v>512.83339999999998</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-89.520380000000003</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.47961999999999705</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>0.40849000000001467</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="3"/>
+        <v>512.83339999999998</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="4"/>
+        <v>7.1294954614718933E-3</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="6"/>
+        <v>1.1334866294151947E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -797,7 +1702,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -821,7 +1726,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="5">
         <v>67</v>
@@ -852,6 +1757,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5500,7 +6406,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6432,10 +7338,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A51BA204-7F14-4F48-A65D-48514DC4DF61}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6446,9 +7352,10 @@
     <col min="6" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -6459,7 +7366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -6469,6 +7376,9 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
       <c r="E2" t="s">
         <v>4</v>
       </c>
@@ -6478,6 +7388,9 @@
       <c r="G2" t="s">
         <v>9</v>
       </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
       <c r="I2" t="s">
         <v>4</v>
       </c>
@@ -6487,8 +7400,20 @@
       <c r="K2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>412</v>
       </c>
@@ -6498,7 +7423,10 @@
       <c r="C3" s="2">
         <v>-113.6665</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2">
+        <f>-90-C3</f>
+        <v>23.666499999999999</v>
+      </c>
       <c r="E3" s="2">
         <v>412</v>
       </c>
@@ -6508,7 +7436,10 @@
       <c r="G3" s="2">
         <v>-107.5153</v>
       </c>
-      <c r="H3" s="2"/>
+      <c r="H3" s="2">
+        <f>-90-G3</f>
+        <v>17.515299999999996</v>
+      </c>
       <c r="I3" s="2">
         <v>11934</v>
       </c>
@@ -6518,8 +7449,28 @@
       <c r="K3" s="2">
         <v>-93.314999999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <f>(D3+H3)/2-$J$8</f>
+        <v>20.217459999999996</v>
+      </c>
+      <c r="M3" s="2">
+        <f>F3</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f>RADIANS(L3)</f>
+        <v>0.35286124339025271</v>
+      </c>
+      <c r="O3">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P3">
+        <f>RADIANS(D3/2-H3/2)</f>
+        <v>5.3679346474337628E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1523</v>
       </c>
@@ -6529,7 +7480,10 @@
       <c r="C4" s="2">
         <v>-108.9589</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D17" si="0">-90-C4</f>
+        <v>18.9589</v>
+      </c>
       <c r="E4" s="2">
         <v>1523</v>
       </c>
@@ -6539,7 +7493,10 @@
       <c r="G4" s="2">
         <v>-103.8544</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4:H17" si="1">-90-G4</f>
+        <v>13.854399999999998</v>
+      </c>
       <c r="I4" s="2">
         <v>11952</v>
       </c>
@@ -6549,8 +7506,28 @@
       <c r="K4" s="2">
         <v>-87.058440000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f t="shared" ref="L4:L17" si="2">(D4+H4)/2-$J$8</f>
+        <v>16.033209999999997</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" ref="M4:M17" si="3">F4</f>
+        <v>37.036830000000002</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N16" si="4">RADIANS(L4)</f>
+        <v>0.27983230416367999</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O16" si="5">1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P16" si="6">RADIANS(D4/2-H4/2)</f>
+        <v>4.4545165834025291E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2592</v>
       </c>
@@ -6560,7 +7537,10 @@
       <c r="C5" s="2">
         <v>-105.7448</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>15.744799999999998</v>
+      </c>
       <c r="E5" s="2">
         <v>2592</v>
       </c>
@@ -6570,12 +7550,37 @@
       <c r="G5" s="2">
         <v>-101.03019999999999</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <f t="shared" si="1"/>
+        <v>11.030199999999994</v>
+      </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>13.014059999999994</v>
+      </c>
+      <c r="M5" s="2">
+        <f t="shared" si="3"/>
+        <v>72.673770000000005</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="4"/>
+        <v>0.22713819605209312</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="6"/>
+        <v>4.1142646457262365E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3660</v>
       </c>
@@ -6585,7 +7590,10 @@
       <c r="C6" s="2">
         <v>-102.9385</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>12.938500000000005</v>
+      </c>
       <c r="E6" s="2">
         <v>3660</v>
       </c>
@@ -6595,12 +7603,38 @@
       <c r="G6" s="2">
         <v>-98.936520000000002</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <f t="shared" si="1"/>
+        <v>8.9365200000000016</v>
+      </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2">
+        <f>-90-K3</f>
+        <v>3.3149999999999977</v>
+      </c>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>10.564070000000001</v>
+      </c>
+      <c r="M6" s="2">
+        <f t="shared" si="3"/>
+        <v>108.27719999999999</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>0.18437780391115738</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="6"/>
+        <v>3.4923863799481362E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>4763</v>
       </c>
@@ -6610,7 +7644,10 @@
       <c r="C7" s="2">
         <v>-100.64960000000001</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>10.649600000000007</v>
+      </c>
       <c r="E7" s="2">
         <v>4763</v>
       </c>
@@ -6620,12 +7657,38 @@
       <c r="G7" s="2">
         <v>-97.132570000000001</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <f t="shared" si="1"/>
+        <v>7.1325700000000012</v>
+      </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="J7" s="2">
+        <f>90+K4</f>
+        <v>2.9415599999999955</v>
+      </c>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>8.5176450000000017</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="3"/>
+        <v>145.04750000000001</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>0.14866094976603245</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="6"/>
+        <v>3.0691876695708133E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>5829</v>
       </c>
@@ -6635,7 +7698,10 @@
       <c r="C8" s="2">
         <v>-98.979439999999997</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>8.9794399999999968</v>
+      </c>
       <c r="E8" s="2">
         <v>5829</v>
       </c>
@@ -6645,12 +7711,38 @@
       <c r="G8" s="2">
         <v>-95.854910000000004</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>5.8549100000000038</v>
+      </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2">
+        <f>J6-J7</f>
+        <v>0.37344000000000221</v>
+      </c>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>7.0437349999999981</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="3"/>
+        <v>180.58430000000001</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>0.12293636738796275</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="6"/>
+        <v>2.7266668038669152E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>6930</v>
       </c>
@@ -6660,7 +7752,10 @@
       <c r="C9" s="2">
         <v>-97.435239999999993</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4352399999999932</v>
+      </c>
       <c r="E9" s="2">
         <v>6930</v>
       </c>
@@ -6670,12 +7765,35 @@
       <c r="G9" s="2">
         <v>-94.703000000000003</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>4.703000000000003</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>5.6956799999999959</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="3"/>
+        <v>217.28790000000001</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>9.9408369139990557E-2</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>2.384329197734485E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>7995</v>
       </c>
@@ -6685,7 +7803,10 @@
       <c r="C10" s="2">
         <v>-96.221500000000006</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>6.221500000000006</v>
+      </c>
       <c r="E10" s="2">
         <v>7995</v>
       </c>
@@ -6695,12 +7816,35 @@
       <c r="G10" s="2">
         <v>-93.649900000000002</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>3.6499000000000024</v>
+      </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>4.562260000000002</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="3"/>
+        <v>252.79140000000001</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>7.9626458332036534E-2</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="6"/>
+        <v>2.2441443522143122E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9096</v>
       </c>
@@ -6710,7 +7854,10 @@
       <c r="C11" s="2">
         <v>-95.193489999999997</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>5.1934899999999971</v>
+      </c>
       <c r="E11" s="2">
         <v>9096</v>
       </c>
@@ -6720,12 +7867,35 @@
       <c r="G11" s="2">
         <v>-93.033010000000004</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>3.0330100000000044</v>
+      </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>3.7398099999999985</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="3"/>
+        <v>289.49489999999997</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>6.5271997899009115E-2</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="6"/>
+        <v>1.8853744711743482E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10161</v>
       </c>
@@ -6735,7 +7905,10 @@
       <c r="C12" s="2">
         <v>-94.152150000000006</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>4.152150000000006</v>
+      </c>
       <c r="E12" s="2">
         <v>10161</v>
       </c>
@@ -6745,12 +7918,35 @@
       <c r="G12" s="2">
         <v>-92.400109999999998</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>2.400109999999998</v>
+      </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>2.9026899999999998</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="3"/>
+        <v>324.9984</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>5.06614976647142E-2</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="6"/>
+        <v>1.5289433313320796E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11260</v>
       </c>
@@ -6760,7 +7956,10 @@
       <c r="C13" s="2">
         <v>-93.816720000000004</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8167200000000037</v>
+      </c>
       <c r="E13" s="2">
         <v>11260</v>
       </c>
@@ -6770,12 +7969,35 @@
       <c r="G13" s="2">
         <v>-91.919759999999997</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.9197599999999966</v>
+      </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>2.4947999999999979</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="3"/>
+        <v>361.63529999999997</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>4.3542474178754495E-2</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="6"/>
+        <v>1.6554098889315878E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12325</v>
       </c>
@@ -6785,7 +8007,10 @@
       <c r="C14" s="2">
         <v>-93.406440000000003</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4064400000000035</v>
+      </c>
       <c r="E14" s="2">
         <v>12325</v>
       </c>
@@ -6795,12 +8020,35 @@
       <c r="G14" s="2">
         <v>-91.426119999999997</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.4261199999999974</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>2.0428399999999982</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="3"/>
+        <v>397.1388</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="4"/>
+        <v>3.5654284091440933E-2</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="6"/>
+        <v>1.7281552121547108E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13424</v>
       </c>
@@ -6810,7 +8058,10 @@
       <c r="C15" s="2">
         <v>-92.720460000000003</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>2.7204600000000028</v>
+      </c>
       <c r="E15" s="2">
         <v>13424</v>
       </c>
@@ -6820,12 +8071,35 @@
       <c r="G15" s="2">
         <v>-91.133080000000007</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1330800000000067</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>1.5533300000000025</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="3"/>
+        <v>433.77569999999997</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="4"/>
+        <v>2.7110722870003563E-2</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="6"/>
+        <v>1.385250374015376E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14487</v>
       </c>
@@ -6835,7 +8109,10 @@
       <c r="C16" s="2">
         <v>-92.444590000000005</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>2.4445900000000051</v>
+      </c>
       <c r="E16" s="2">
         <v>14487</v>
       </c>
@@ -6845,12 +8122,35 @@
       <c r="G16" s="2">
         <v>-90.809979999999996</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.80997999999999593</v>
+      </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>1.2538449999999983</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="3"/>
+        <v>469.21249999999998</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>2.1883723559668271E-2</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="5"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="6"/>
+        <v>1.4264663243012336E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15587</v>
       </c>
@@ -6860,7 +8160,10 @@
       <c r="C17" s="2">
         <v>-92.127300000000005</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>2.1273000000000053</v>
+      </c>
       <c r="E17" s="2">
         <v>15587</v>
       </c>
@@ -6870,12 +8173,35 @@
       <c r="G17" s="2">
         <v>-90.555160000000001</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.55516000000000076</v>
+      </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>0.96779000000000082</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="3"/>
+        <v>505.8827</v>
+      </c>
+      <c r="N17">
+        <f>RADIANS(L17)</f>
+        <v>1.6891121967875938E-2</v>
+      </c>
+      <c r="O17">
+        <f>1/30</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="P17">
+        <f>RADIANS(D17/2-H17/2)</f>
+        <v>1.3719509651151866E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -6885,7 +8211,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -6909,7 +8235,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="5">
         <v>452</v>
@@ -6948,7 +8274,7 @@
   <dimension ref="A24:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:H26"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7021,5 +8347,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started writing v2 lab
</commit_message>
<xml_diff>
--- a/plotting/raw_retake.xlsx
+++ b/plotting/raw_retake.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\GitHub\Togohogo1-Archive\phy180-pendulum-report\plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F63BF9B-ACD1-447F-85A4-173011EE2DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4893699D-CDF9-445A-912D-0CECFF620EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="local" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="len7" sheetId="5" r:id="rId8"/>
     <sheet name="len8" sheetId="6" r:id="rId9"/>
     <sheet name="len9" sheetId="7" r:id="rId10"/>
+    <sheet name="Q" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -79,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="37">
   <si>
     <t>t</t>
   </si>
@@ -179,6 +180,18 @@
   <si>
     <t>thetaf</t>
   </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>dL</t>
+  </si>
+  <si>
+    <t>dQ</t>
+  </si>
 </sst>
 </file>
 
@@ -246,16 +259,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,9 +552,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -564,7 +574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4.3</v>
       </c>
@@ -588,7 +598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4.5999999999999996</v>
       </c>
@@ -609,7 +619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4.5</v>
       </c>
@@ -634,7 +644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4.5</v>
       </c>
@@ -655,7 +665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4.5</v>
       </c>
@@ -680,7 +690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4.5</v>
       </c>
@@ -701,7 +711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4.5</v>
       </c>
@@ -725,7 +735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4.5</v>
       </c>
@@ -746,7 +756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>4.5</v>
       </c>
@@ -780,23 +790,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8740C19F-6777-4FB3-9718-68300DD6568C}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -808,7 +818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -855,7 +865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>355</v>
       </c>
@@ -912,7 +922,7 @@
         <v>8.0388120017606798E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1577</v>
       </c>
@@ -969,7 +979,7 @@
         <v>6.3343234542630217E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2796</v>
       </c>
@@ -1020,7 +1030,7 @@
         <v>4.8082162829654398E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4013</v>
       </c>
@@ -1074,7 +1084,7 @@
         <v>3.7370989943702672E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5228</v>
       </c>
@@ -1128,7 +1138,7 @@
         <v>2.8463789372612069E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6444</v>
       </c>
@@ -1182,7 +1192,7 @@
         <v>2.2296668460690124E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7658</v>
       </c>
@@ -1235,7 +1245,7 @@
         <v>2.0744808956279365E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8874</v>
       </c>
@@ -1286,7 +1296,7 @@
         <v>1.6014792150449587E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10087</v>
       </c>
@@ -1337,7 +1347,7 @@
         <v>1.5708486866724582E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11302</v>
       </c>
@@ -1388,7 +1398,7 @@
         <v>1.3673694758286982E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12515</v>
       </c>
@@ -1439,7 +1449,7 @@
         <v>1.5054337463077069E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13728</v>
       </c>
@@ -1490,7 +1500,7 @@
         <v>1.2523697314147987E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14942</v>
       </c>
@@ -1541,7 +1551,7 @@
         <v>1.2716294397105556E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>16156</v>
       </c>
@@ -1592,7 +1602,7 @@
         <v>1.5177819507655675E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>17368</v>
       </c>
@@ -1643,7 +1653,7 @@
         <v>1.5675412877399333E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -1653,7 +1663,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -1677,7 +1687,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="4">
         <v>397</v>
@@ -1712,26 +1722,262 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499598B7-F26E-4D5F-8D5D-5BBABBF2DBCA}">
+  <dimension ref="B1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12:L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>10.95</v>
+      </c>
+      <c r="C2">
+        <v>343.06737984429299</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>12.9249727332402</v>
+      </c>
+      <c r="G2">
+        <v>10.95</v>
+      </c>
+      <c r="H2">
+        <v>353.39820590050999</v>
+      </c>
+      <c r="I2">
+        <v>14.848624978188701</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="C3">
+        <v>463.79441737610898</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3">
+        <v>16.4200121751918</v>
+      </c>
+      <c r="G3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="H3">
+        <v>478.89203540698401</v>
+      </c>
+      <c r="I3">
+        <v>18.157320998629</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>20.75</v>
+      </c>
+      <c r="C4">
+        <v>514.06112114718997</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4">
+        <v>10.5269065704812</v>
+      </c>
+      <c r="G4">
+        <v>20.75</v>
+      </c>
+      <c r="H4">
+        <v>534.18331144129002</v>
+      </c>
+      <c r="I4">
+        <v>7.2278937308355697</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>24.3</v>
+      </c>
+      <c r="C5">
+        <v>463.285583147083</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5">
+        <v>9.5444804514781403</v>
+      </c>
+      <c r="G5">
+        <v>24.3</v>
+      </c>
+      <c r="H5">
+        <v>485.269929738386</v>
+      </c>
+      <c r="I5">
+        <v>8.3624071969841705</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>30.1</v>
+      </c>
+      <c r="C6">
+        <v>479.87190472681999</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+      <c r="E6">
+        <v>5.1828034116898696</v>
+      </c>
+      <c r="G6">
+        <v>30.1</v>
+      </c>
+      <c r="H6">
+        <v>483.74930013802299</v>
+      </c>
+      <c r="I6">
+        <v>7.2640930171459104</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>34.6</v>
+      </c>
+      <c r="C7">
+        <v>465.62990611073502</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="E7">
+        <v>2.9760194487037901</v>
+      </c>
+      <c r="G7">
+        <v>34.6</v>
+      </c>
+      <c r="H7">
+        <v>460.03104027910899</v>
+      </c>
+      <c r="I7">
+        <v>3.02030759327145</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="C8">
+        <v>444.57233800827998</v>
+      </c>
+      <c r="D8">
+        <v>0.1</v>
+      </c>
+      <c r="E8">
+        <v>8.6412964993168</v>
+      </c>
+      <c r="G8">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="H8">
+        <v>432.23994693613997</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>42.8</v>
+      </c>
+      <c r="C9">
+        <v>422.14563967364398</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+      <c r="E9">
+        <v>9.3728953070143994</v>
+      </c>
+      <c r="G9">
+        <v>42.8</v>
+      </c>
+      <c r="H9">
+        <v>407.24129782379202</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>48.8</v>
+      </c>
+      <c r="C10">
+        <v>430.74108669930598</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10">
+        <v>20.814407894632499</v>
+      </c>
+      <c r="G10">
+        <v>48.8</v>
+      </c>
+      <c r="H10">
+        <v>395.16759574716099</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:P22"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9:P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -1742,7 +1988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1786,7 +2032,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>218</v>
       </c>
@@ -1835,8 +2081,9 @@
         <f>RADIANS((D3-H3)/2)</f>
         <v>1.4351842439149345E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R3" s="2"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>668</v>
       </c>
@@ -1885,8 +2132,12 @@
         <f t="shared" ref="P4:P22" si="5">RADIANS((D4-H4)/2)</f>
         <v>1.1623020153656276E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R4" s="2">
+        <f>N3-N4</f>
+        <v>3.9680933208716962E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1116</v>
       </c>
@@ -1935,8 +2186,12 @@
         <f t="shared" si="5"/>
         <v>1.2941616403537989E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R5" s="2">
+        <f t="shared" ref="R5:R22" si="6">N4-N5</f>
+        <v>4.9236610863386154E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1564</v>
       </c>
@@ -1985,8 +2240,12 @@
         <f t="shared" si="5"/>
         <v>1.4474015486788911E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R6" s="2">
+        <f t="shared" si="6"/>
+        <v>4.1378265906281492E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2011</v>
       </c>
@@ -2036,8 +2295,12 @@
         <f t="shared" si="5"/>
         <v>1.210734902108466E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R7" s="2">
+        <f t="shared" si="6"/>
+        <v>3.6686820876920878E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2458</v>
       </c>
@@ -2087,8 +2350,12 @@
         <f t="shared" si="5"/>
         <v>8.4583018874775408E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R8" s="2">
+        <f t="shared" si="6"/>
+        <v>3.3066920741821881E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>2924</v>
       </c>
@@ -2138,8 +2405,12 @@
         <f t="shared" si="5"/>
         <v>1.0399020749232673E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R9" s="2">
+        <f t="shared" si="6"/>
+        <v>3.0160773004326208E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>3370</v>
       </c>
@@ -2185,8 +2456,12 @@
         <f t="shared" si="5"/>
         <v>1.0561510902593208E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R10" s="2">
+        <f t="shared" si="6"/>
+        <v>3.0304675401153197E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>3815</v>
       </c>
@@ -2232,8 +2507,12 @@
         <f t="shared" si="5"/>
         <v>1.202793654011901E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R11" s="2">
+        <f t="shared" si="6"/>
+        <v>1.7757328875640729E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>4260</v>
       </c>
@@ -2279,8 +2558,12 @@
         <f t="shared" si="5"/>
         <v>1.0931957036329024E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R12" s="2">
+        <f t="shared" si="6"/>
+        <v>2.087562138371632E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>4725</v>
       </c>
@@ -2326,8 +2609,12 @@
         <f t="shared" si="5"/>
         <v>1.0450595228629105E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R13" s="2">
+        <f t="shared" si="6"/>
+        <v>1.1300134242037269E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>5169</v>
       </c>
@@ -2373,8 +2660,12 @@
         <f t="shared" si="5"/>
         <v>1.0450071629853465E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R14" s="2">
+        <f t="shared" si="6"/>
+        <v>1.6823403192898642E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>5612</v>
       </c>
@@ -2420,8 +2711,12 @@
         <f t="shared" si="5"/>
         <v>9.5215564677925378E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R15" s="2">
+        <f t="shared" si="6"/>
+        <v>8.592604973418471E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>6076</v>
       </c>
@@ -2467,8 +2762,12 @@
         <f t="shared" si="5"/>
         <v>8.0088796050889633E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R16" s="2">
+        <f t="shared" si="6"/>
+        <v>5.8716366695592687E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>6518</v>
       </c>
@@ -2514,8 +2813,12 @@
         <f t="shared" si="5"/>
         <v>9.6359628002607445E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R17" s="2">
+        <f t="shared" si="6"/>
+        <v>5.6244107810142982E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>6961</v>
       </c>
@@ -2561,8 +2864,12 @@
         <f t="shared" si="5"/>
         <v>9.5386606944620547E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R18" s="2">
+        <f t="shared" si="6"/>
+        <v>1.7846864266269184E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>7422</v>
       </c>
@@ -2608,8 +2915,12 @@
         <f t="shared" si="5"/>
         <v>1.0139490289461083E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R19" s="2">
+        <f t="shared" si="6"/>
+        <v>3.9598902733872614E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>7863</v>
       </c>
@@ -2655,8 +2966,12 @@
         <f t="shared" si="5"/>
         <v>9.2080953341343186E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R20" s="2">
+        <f t="shared" si="6"/>
+        <v>8.2527893680555721E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>8325</v>
       </c>
@@ -2702,8 +3017,12 @@
         <f t="shared" si="5"/>
         <v>8.8325877455676001E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R21" s="2">
+        <f t="shared" si="6"/>
+        <v>1.753270500090845E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>8765</v>
       </c>
@@ -2749,13 +3068,17 @@
         <f t="shared" si="5"/>
         <v>9.4666658628172543E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R22" s="2">
+        <f t="shared" si="6"/>
+        <v>1.1613420842770861E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>239</v>
       </c>
@@ -2775,7 +3098,7 @@
         <v>0.68666666666666676</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>19</v>
       </c>
@@ -2795,22 +3118,22 @@
       <selection activeCell="N2" sqref="N2:Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -2821,7 +3144,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2871,7 +3194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>219</v>
       </c>
@@ -2928,7 +3251,7 @@
         <v>1.640173164561665E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1190</v>
       </c>
@@ -2985,7 +3308,7 @@
         <v>1.8719528892265174E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2157</v>
       </c>
@@ -3036,7 +3359,7 @@
         <v>1.2616985162667056E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>3148</v>
       </c>
@@ -3090,7 +3413,7 @@
         <v>1.1741702542791863E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>4112</v>
       </c>
@@ -3144,7 +3467,7 @@
         <v>1.1103435635337455E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>5075</v>
       </c>
@@ -3198,7 +3521,7 @@
         <v>1.1620489426240827E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>6061</v>
       </c>
@@ -3249,7 +3572,7 @@
         <v>1.0319171935953886E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>7023</v>
       </c>
@@ -3300,7 +3623,7 @@
         <v>1.0915027342584762E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>7983</v>
       </c>
@@ -3351,7 +3674,7 @@
         <v>1.2126809442244374E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>8968</v>
       </c>
@@ -3402,7 +3725,7 @@
         <v>9.9898283061025609E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>9926</v>
       </c>
@@ -3453,7 +3776,7 @@
         <v>1.2360683562011565E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>10908</v>
       </c>
@@ -3504,7 +3827,7 @@
         <v>9.4463327770315155E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>11865</v>
       </c>
@@ -3555,7 +3878,7 @@
         <v>1.2743259734048872E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>12845</v>
       </c>
@@ -3606,7 +3929,7 @@
         <v>1.1622496554880637E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>13824</v>
       </c>
@@ -3657,7 +3980,7 @@
         <v>1.0094198995371839E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -3667,7 +3990,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -3691,7 +4014,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="4">
         <v>244</v>
@@ -3734,24 +4057,24 @@
       <selection activeCell="M2" sqref="M2:P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="1"/>
+    <col min="9" max="9" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.26953125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="9.1796875" style="1"/>
+    <col min="14" max="14" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -3765,7 +4088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3806,7 +4129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>209</v>
       </c>
@@ -3859,7 +4182,7 @@
         <v>2.1314833489980835E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1152</v>
       </c>
@@ -3912,7 +4235,7 @@
         <v>1.5928747418326235E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2065</v>
       </c>
@@ -3962,7 +4285,7 @@
         <v>1.2749630185818565E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>3003</v>
       </c>
@@ -4013,7 +4336,7 @@
         <v>1.0797479417462837E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>3940</v>
       </c>
@@ -4064,7 +4387,7 @@
         <v>1.0824532020868778E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>4848</v>
       </c>
@@ -4115,7 +4438,7 @@
         <v>1.6174489777007035E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>5783</v>
       </c>
@@ -4162,7 +4485,7 @@
         <v>1.5263864239779023E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>6718</v>
       </c>
@@ -4209,7 +4532,7 @@
         <v>1.4231676520149589E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>7651</v>
       </c>
@@ -4256,7 +4579,7 @@
         <v>1.3859223257773962E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>8585</v>
       </c>
@@ -4303,7 +4626,7 @@
         <v>1.4931379017274104E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>9517</v>
       </c>
@@ -4350,7 +4673,7 @@
         <v>1.6320661101861575E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>10450</v>
       </c>
@@ -4397,7 +4720,7 @@
         <v>1.3734606749181573E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>11382</v>
       </c>
@@ -4444,7 +4767,7 @@
         <v>1.6639358223275828E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>12313</v>
       </c>
@@ -4491,7 +4814,7 @@
         <v>1.1792578890487401E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>13244</v>
       </c>
@@ -4538,12 +4861,12 @@
         <v>1.1403894066068282E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
@@ -4560,7 +4883,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B26" s="1">
         <v>1057</v>
       </c>
@@ -4593,33 +4916,31 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>5</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4644,13 +4965,13 @@
       <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" t="s">
         <v>9</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -4666,7 +4987,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>35</v>
       </c>
@@ -4693,13 +5014,13 @@
         <f>-90-G3</f>
         <v>17.031499999999994</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="2">
         <v>7998</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="2">
         <v>265.44260000000003</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="2">
         <v>-94.269499999999994</v>
       </c>
       <c r="L3">
@@ -4723,7 +5044,7 @@
         <v>4.2161046075801012E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>1055</v>
       </c>
@@ -4750,13 +5071,13 @@
         <f t="shared" ref="H4:H18" si="1">-90-G4</f>
         <v>13.492099999999994</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="2">
         <v>8014</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="2">
         <v>265.976</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="2">
         <v>-85.491829999999993</v>
       </c>
       <c r="L4">
@@ -4780,7 +5101,7 @@
         <v>3.868347754120232E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2101</v>
       </c>
@@ -4807,8 +5128,8 @@
         <f t="shared" si="1"/>
         <v>10.850200000000001</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5">
         <f t="shared" si="2"/>
@@ -4831,7 +5152,7 @@
         <v>3.3231941622597995E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>3116</v>
       </c>
@@ -4858,8 +5179,8 @@
         <f t="shared" si="1"/>
         <v>8.5662099999999981</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
         <f>-90-K3</f>
         <v>4.2694999999999936</v>
       </c>
@@ -4885,7 +5206,7 @@
         <v>3.0671456343459764E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>4159</v>
       </c>
@@ -4912,8 +5233,8 @@
         <f t="shared" si="1"/>
         <v>6.7177999999999969</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2">
         <f>-90-K4</f>
         <v>-4.5081700000000069</v>
       </c>
@@ -4939,7 +5260,7 @@
         <v>2.7599851392874967E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>5172</v>
       </c>
@@ -4966,8 +5287,8 @@
         <f t="shared" si="1"/>
         <v>5.404049999999998</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2">
         <f>AVERAGE(J6:J7)</f>
         <v>-0.11933500000000663</v>
       </c>
@@ -4993,7 +5314,7 @@
         <v>2.339125170107844E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>6214</v>
       </c>
@@ -5020,8 +5341,8 @@
         <f t="shared" si="1"/>
         <v>4.0910899999999941</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
       <c r="K9" s="2" t="s">
         <v>29</v>
       </c>
@@ -5046,7 +5367,7 @@
         <v>2.1199205427036214E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>7226</v>
       </c>
@@ -5073,8 +5394,8 @@
         <f t="shared" si="1"/>
         <v>3.0318199999999962</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10">
         <f t="shared" si="2"/>
@@ -5097,7 +5418,7 @@
         <v>1.9233266557589696E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>8267</v>
       </c>
@@ -5124,8 +5445,8 @@
         <f t="shared" si="1"/>
         <v>2.0566199999999952</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11">
         <f t="shared" si="2"/>
@@ -5148,7 +5469,7 @@
         <v>1.8241657743069236E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>9278</v>
       </c>
@@ -5175,8 +5496,8 @@
         <f t="shared" si="1"/>
         <v>1.321780000000004</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12">
         <f t="shared" si="2"/>
@@ -5199,7 +5520,7 @@
         <v>1.7414197144698614E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>10318</v>
       </c>
@@ -5226,8 +5547,8 @@
         <f t="shared" si="1"/>
         <v>0.77075999999999567</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13">
         <f t="shared" si="2"/>
@@ -5250,7 +5571,7 @@
         <v>1.7159640873295297E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>11357</v>
       </c>
@@ -5277,8 +5598,8 @@
         <f t="shared" si="1"/>
         <v>0.39548999999999523</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14">
         <f t="shared" si="2"/>
@@ -5301,7 +5622,7 @@
         <v>1.5718697042848766E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>12366</v>
       </c>
@@ -5328,8 +5649,8 @@
         <f t="shared" si="1"/>
         <v>0.14101999999999748</v>
       </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15">
         <f t="shared" si="2"/>
@@ -5352,7 +5673,7 @@
         <v>1.3685650263663217E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>13405</v>
       </c>
@@ -5379,8 +5700,8 @@
         <f t="shared" si="1"/>
         <v>0.13430999999999926</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16">
         <f t="shared" si="2"/>
@@ -5403,7 +5724,7 @@
         <v>1.2647702957502109E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>14443</v>
       </c>
@@ -5430,8 +5751,8 @@
         <f t="shared" si="1"/>
         <v>-6.3700000000039836E-3</v>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17">
         <f t="shared" si="2"/>
@@ -5454,7 +5775,7 @@
         <v>1.0111390488503983E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>15419</v>
       </c>
@@ -5481,8 +5802,8 @@
         <f t="shared" si="1"/>
         <v>-0.47961999999999705</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18">
         <f t="shared" si="2"/>
@@ -5505,7 +5826,7 @@
         <v>1.1334866294151947E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -5515,7 +5836,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -5539,7 +5860,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="4">
         <v>67</v>
@@ -5582,23 +5903,23 @@
       <selection activeCell="N2" sqref="N2:Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="1"/>
-    <col min="9" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7109375" style="1"/>
+    <col min="8" max="8" width="8.7265625" style="1"/>
+    <col min="9" max="10" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -5609,7 +5930,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -5659,7 +5980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>387</v>
       </c>
@@ -5715,7 +6036,7 @@
         <v>4.2529310547971766E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1482</v>
       </c>
@@ -5771,7 +6092,7 @@
         <v>3.6655404950384926E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2540</v>
       </c>
@@ -5821,7 +6142,7 @@
         <v>3.0737866121498147E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>3630</v>
       </c>
@@ -5872,7 +6193,7 @@
         <v>2.5806438319988158E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>4719</v>
       </c>
@@ -5923,7 +6244,7 @@
         <v>2.0882777233649532E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>5807</v>
       </c>
@@ -5974,7 +6295,7 @@
         <v>1.9980442010368395E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>6860</v>
       </c>
@@ -6021,7 +6342,7 @@
         <v>1.6013832219360931E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>7947</v>
       </c>
@@ -6068,7 +6389,7 @@
         <v>1.5342404056118648E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9033</v>
       </c>
@@ -6115,7 +6436,7 @@
         <v>1.1478681424516291E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10120</v>
       </c>
@@ -6162,7 +6483,7 @@
         <v>1.5474874546345149E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11204</v>
       </c>
@@ -6209,7 +6530,7 @@
         <v>1.5069696360494657E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12290</v>
       </c>
@@ -6256,7 +6577,7 @@
         <v>1.3727014566935343E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13375</v>
       </c>
@@ -6303,7 +6624,7 @@
         <v>1.0569452150689822E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14425</v>
       </c>
@@ -6350,7 +6671,7 @@
         <v>1.2487830798019406E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15511</v>
       </c>
@@ -6397,7 +6718,7 @@
         <v>1.1400927006339942E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16199</v>
       </c>
@@ -6444,12 +6765,12 @@
         <v>1.2742736135273231E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
@@ -6466,7 +6787,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B26" s="1">
         <v>420</v>
       </c>
@@ -6499,18 +6820,18 @@
       <selection activeCell="M2" sqref="M2:P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -6521,7 +6842,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -6568,7 +6889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>412</v>
       </c>
@@ -6625,7 +6946,7 @@
         <v>5.3679346474337628E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>1523</v>
       </c>
@@ -6682,7 +7003,7 @@
         <v>4.4545165834025291E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2592</v>
       </c>
@@ -6735,7 +7056,7 @@
         <v>4.1142646457262365E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>3660</v>
       </c>
@@ -6789,7 +7110,7 @@
         <v>3.4923863799481362E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>4763</v>
       </c>
@@ -6843,7 +7164,7 @@
         <v>3.0691876695708133E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>5829</v>
       </c>
@@ -6897,7 +7218,7 @@
         <v>2.7266668038669152E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>6930</v>
       </c>
@@ -6948,7 +7269,7 @@
         <v>2.384329197734485E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>7995</v>
       </c>
@@ -6999,7 +7320,7 @@
         <v>2.2441443522143122E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>9096</v>
       </c>
@@ -7050,7 +7371,7 @@
         <v>1.8853744711743482E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>10161</v>
       </c>
@@ -7101,7 +7422,7 @@
         <v>1.5289433313320796E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>11260</v>
       </c>
@@ -7152,7 +7473,7 @@
         <v>1.6554098889315878E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>12325</v>
       </c>
@@ -7203,7 +7524,7 @@
         <v>1.7281552121547108E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>13424</v>
       </c>
@@ -7254,7 +7575,7 @@
         <v>1.385250374015376E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>14487</v>
       </c>
@@ -7305,7 +7626,7 @@
         <v>1.4264663243012336E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>15587</v>
       </c>
@@ -7356,7 +7677,7 @@
         <v>1.3719509651151866E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -7366,7 +7687,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -7390,7 +7711,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="4">
         <v>452</v>
@@ -7432,19 +7753,19 @@
       <selection activeCell="M2" sqref="M2:P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -7455,7 +7776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -7502,7 +7823,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>96</v>
       </c>
@@ -7556,7 +7877,7 @@
         <v>6.2477551233641057E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1344</v>
       </c>
@@ -7610,7 +7931,7 @@
         <v>5.1164327022213768E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2627</v>
       </c>
@@ -7661,7 +7982,7 @@
         <v>4.2736917462496533E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>3869</v>
       </c>
@@ -7713,7 +8034,7 @@
         <v>3.5241077391031321E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5149</v>
       </c>
@@ -7765,7 +8086,7 @@
         <v>2.9592755599264674E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6390</v>
       </c>
@@ -7817,7 +8138,7 @@
         <v>2.4541772743993075E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7667</v>
       </c>
@@ -7865,7 +8186,7 @@
         <v>2.1128519592330332E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8907</v>
       </c>
@@ -7913,7 +8234,7 @@
         <v>1.9467489743207275E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10184</v>
       </c>
@@ -7961,7 +8282,7 @@
         <v>1.7375538101766945E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11422</v>
       </c>
@@ -8009,7 +8330,7 @@
         <v>1.4440854231001036E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12700</v>
       </c>
@@ -8057,7 +8378,7 @@
         <v>1.3212142437597038E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13938</v>
       </c>
@@ -8105,7 +8426,7 @@
         <v>1.415968168850479E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>15214</v>
       </c>
@@ -8153,7 +8474,7 @@
         <v>1.4605700578851889E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>16451</v>
       </c>
@@ -8201,7 +8522,7 @@
         <v>1.0200489546818176E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>17727</v>
       </c>
@@ -8249,7 +8570,7 @@
         <v>1.0565176094022443E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -8259,7 +8580,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -8283,7 +8604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1">
         <v>134</v>
@@ -8325,21 +8646,21 @@
       <selection activeCell="L2" sqref="L2:O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -8350,7 +8671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -8397,7 +8718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>428</v>
       </c>
@@ -8451,7 +8772,7 @@
         <v>7.954163533038959E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1697</v>
       </c>
@@ -8505,7 +8826,7 @@
         <v>5.9559360724306523E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2962</v>
       </c>
@@ -8556,7 +8877,7 @@
         <v>5.1622301417937104E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4223</v>
       </c>
@@ -8612,7 +8933,7 @@
         <v>4.2858305111972701E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5446</v>
       </c>
@@ -8664,7 +8985,7 @@
         <v>3.9279420214295827E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6707</v>
       </c>
@@ -8712,7 +9033,7 @@
         <v>3.5166988164284083E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7968</v>
       </c>
@@ -8760,7 +9081,7 @@
         <v>3.2248448589099282E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9228</v>
       </c>
@@ -8808,7 +9129,7 @@
         <v>2.3044280245781958E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10487</v>
       </c>
@@ -8856,7 +9177,7 @@
         <v>2.1986610719073381E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11748</v>
       </c>
@@ -8904,7 +9225,7 @@
         <v>1.876761271315763E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>13006</v>
       </c>
@@ -8952,7 +9273,7 @@
         <v>1.8102467735222533E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>14264</v>
       </c>
@@ -9000,7 +9321,7 @@
         <v>1.5312646192372248E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>15563</v>
       </c>
@@ -9048,7 +9369,7 @@
         <v>1.6317170443357596E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>16819</v>
       </c>
@@ -9096,7 +9417,7 @@
         <v>1.4510056535842626E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>18077</v>
       </c>
@@ -9144,7 +9465,7 @@
         <v>1.5330884883055673E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
@@ -9154,7 +9475,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
@@ -9178,7 +9499,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="4">
         <v>468</v>

</xml_diff>

<commit_message>
plot r^2 and equation in legend
</commit_message>
<xml_diff>
--- a/plotting/raw_retake.xlsx
+++ b/plotting/raw_retake.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\GitHub\Togohogo1-Archive\phy180-pendulum-report\plotting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4893699D-CDF9-445A-912D-0CECFF620EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A28ED5-A9F4-468F-9029-22C4DA00C229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="local" sheetId="2" r:id="rId1"/>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8740C19F-6777-4FB3-9718-68300DD6568C}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1726,7 +1726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499598B7-F26E-4D5F-8D5D-5BBABBF2DBCA}">
   <dimension ref="B1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12:L13"/>
     </sheetView>
   </sheetViews>

</xml_diff>